<commit_message>
Integrate new study findings by Wei et al.
</commit_message>
<xml_diff>
--- a/Supplementary_materials/Supplementary Table 2.xlsx
+++ b/Supplementary_materials/Supplementary Table 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonguo/myDocuments/研究生/STAT department documents/MATH 581 directed studies/20201205/论文supplement material/正式/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonguo/myDocuments/git_local_repo/COVIDnetwork/Supplementary_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8E1C660-4DCC-9B47-AA0A-9D32268191F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1451ED8-6364-2643-B7B0-338A917393EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{2EE752A0-736C-C649-8CDE-11D356C6D5DD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="1117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="1118">
   <si>
     <t>P11142</t>
   </si>
@@ -3114,9 +3114,6 @@
     <t>PTGS2 has synonyms COX-2, so search for https://pubmed.ncbi.nlm.nih.gov/?term=%28COX-2%29+AND+COVID-19 returns 19 hits, in which there is 1 preprint: https://pubmed.ncbi.nlm.nih.gov/32995789/; 1 unrelated hit: https://pubmed.ncbi.nlm.nih.gov/32599375/.</t>
   </si>
   <si>
-    <t>Number of connections to 54 SARS-Cov-2 interacting human proteins</t>
-  </si>
-  <si>
     <t>Q15645</t>
   </si>
   <si>
@@ -3385,6 +3382,12 @@
   </si>
   <si>
     <t>Number of hits matched to COVID-19 (as of Dec27 2020, * means additional comments about number of hits)</t>
+  </si>
+  <si>
+    <t>Number of connections to 57 SARS-Cov-2 interacting human proteins</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/34162861/</t>
   </si>
 </sst>
 </file>
@@ -3769,8 +3772,8 @@
   <dimension ref="A1:N334"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H164" sqref="H164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3780,21 +3783,21 @@
     <col min="6" max="6" width="54.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="53" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1114</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>1115</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1116</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>1026</v>
+        <v>1116</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>744</v>
@@ -3814,7 +3817,7 @@
         <v>865</v>
       </c>
       <c r="E2">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -3831,7 +3834,7 @@
         <v>866</v>
       </c>
       <c r="E3">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
         <v>745</v>
@@ -3851,7 +3854,7 @@
         <v>867</v>
       </c>
       <c r="E4">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>746</v>
@@ -3871,7 +3874,7 @@
         <v>868</v>
       </c>
       <c r="E5">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -3888,7 +3891,7 @@
         <v>869</v>
       </c>
       <c r="E6">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -3902,13 +3905,13 @@
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>1110</v>
+      </c>
+      <c r="E7">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
         <v>1111</v>
-      </c>
-      <c r="E7">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -3925,7 +3928,7 @@
         <v>31</v>
       </c>
       <c r="E8">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
         <v>17</v>
@@ -3965,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="E10">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>4</v>
@@ -3985,7 +3988,7 @@
         <v>871</v>
       </c>
       <c r="E11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F11" t="s">
         <v>364</v>
@@ -4010,7 +4013,7 @@
         <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -4027,7 +4030,7 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -4044,7 +4047,7 @@
         <v>873</v>
       </c>
       <c r="E14">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
@@ -4061,7 +4064,7 @@
         <v>13</v>
       </c>
       <c r="E15">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -4075,10 +4078,10 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="E16">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -4112,7 +4115,7 @@
         <v>874</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
         <v>381</v>
@@ -4132,7 +4135,7 @@
         <v>875</v>
       </c>
       <c r="E19">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F19" t="s">
         <v>375</v>
@@ -4152,7 +4155,7 @@
         <v>14</v>
       </c>
       <c r="E20">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F20" t="s">
         <v>17</v>
@@ -4172,7 +4175,7 @@
         <v>19</v>
       </c>
       <c r="E21">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
         <v>17</v>
@@ -4192,7 +4195,7 @@
         <v>876</v>
       </c>
       <c r="E22">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -4209,7 +4212,7 @@
         <v>877</v>
       </c>
       <c r="E23">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -4226,7 +4229,7 @@
         <v>878</v>
       </c>
       <c r="E24">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F24" t="s">
         <v>379</v>
@@ -4246,7 +4249,7 @@
         <v>21</v>
       </c>
       <c r="E25">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -4263,7 +4266,7 @@
         <v>879</v>
       </c>
       <c r="E26">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
         <v>485</v>
@@ -4283,7 +4286,7 @@
         <v>880</v>
       </c>
       <c r="E27">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -4300,7 +4303,7 @@
         <v>25</v>
       </c>
       <c r="E28">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -4334,7 +4337,7 @@
         <v>881</v>
       </c>
       <c r="E30">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -4351,7 +4354,7 @@
         <v>882</v>
       </c>
       <c r="E31">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
         <v>404</v>
@@ -4371,7 +4374,7 @@
         <v>883</v>
       </c>
       <c r="E32">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -4388,7 +4391,7 @@
         <v>31</v>
       </c>
       <c r="E33">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
         <v>30</v>
@@ -4408,7 +4411,7 @@
         <v>35</v>
       </c>
       <c r="E34">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -4425,7 +4428,7 @@
         <v>39</v>
       </c>
       <c r="E35">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F35" t="s">
         <v>17</v>
@@ -4445,7 +4448,7 @@
         <v>884</v>
       </c>
       <c r="E36">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F36" t="s">
         <v>486</v>
@@ -4465,7 +4468,7 @@
         <v>408</v>
       </c>
       <c r="E37">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -4499,7 +4502,7 @@
         <v>886</v>
       </c>
       <c r="E39">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -4533,7 +4536,7 @@
         <v>887</v>
       </c>
       <c r="E41">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -4550,7 +4553,7 @@
         <v>888</v>
       </c>
       <c r="E42">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -4587,7 +4590,7 @@
         <v>890</v>
       </c>
       <c r="E44">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F44" t="s">
         <v>484</v>
@@ -4627,7 +4630,7 @@
         <v>891</v>
       </c>
       <c r="E46">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>413</v>
@@ -4664,7 +4667,7 @@
         <v>892</v>
       </c>
       <c r="E48">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F48" t="s">
         <v>418</v>
@@ -4684,7 +4687,7 @@
         <v>50</v>
       </c>
       <c r="E49">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="F49" t="s">
         <v>17</v>
@@ -4704,7 +4707,7 @@
         <v>893</v>
       </c>
       <c r="E50">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F50" t="s">
         <v>1018</v>
@@ -4724,7 +4727,7 @@
         <v>894</v>
       </c>
       <c r="E51">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F51" t="s">
         <v>655</v>
@@ -4781,7 +4784,7 @@
         <v>57</v>
       </c>
       <c r="E54">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F54" t="s">
         <v>413</v>
@@ -4872,7 +4875,7 @@
         <v>898</v>
       </c>
       <c r="E59">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F59" t="s">
         <v>479</v>
@@ -4912,7 +4915,7 @@
         <v>899</v>
       </c>
       <c r="E61">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F61" t="s">
         <v>480</v>
@@ -4932,7 +4935,7 @@
         <v>900</v>
       </c>
       <c r="E62">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F62" t="s">
         <v>481</v>
@@ -4969,27 +4972,27 @@
         <v>901</v>
       </c>
       <c r="E64">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B65" t="s">
         <v>1055</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1056</v>
       </c>
       <c r="C65" s="4">
         <v>2</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="E65">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
@@ -5026,7 +5029,7 @@
         <v>903</v>
       </c>
       <c r="E67">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F67" t="s">
         <v>482</v>
@@ -5046,7 +5049,7 @@
         <v>71</v>
       </c>
       <c r="E68">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F68" t="s">
         <v>70</v>
@@ -5054,19 +5057,19 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B69" t="s">
         <v>1027</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" s="4">
+        <v>1</v>
+      </c>
+      <c r="D69" s="1" t="s">
         <v>1028</v>
       </c>
-      <c r="C69" s="4">
-        <v>1</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>1029</v>
-      </c>
       <c r="E69">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -5083,7 +5086,7 @@
         <v>904</v>
       </c>
       <c r="E70">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -5100,7 +5103,7 @@
         <v>76</v>
       </c>
       <c r="E71">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F71" t="s">
         <v>17</v>
@@ -5120,7 +5123,7 @@
         <v>80</v>
       </c>
       <c r="E72">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F72" t="s">
         <v>77</v>
@@ -5140,7 +5143,7 @@
         <v>905</v>
       </c>
       <c r="E73">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -5157,7 +5160,7 @@
         <v>82</v>
       </c>
       <c r="E74">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -5194,7 +5197,7 @@
         <v>906</v>
       </c>
       <c r="E76">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F76" t="s">
         <v>457</v>
@@ -5259,19 +5262,19 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B80" t="s">
         <v>1030</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" s="4">
+        <v>1</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>1031</v>
       </c>
-      <c r="C80" s="4">
-        <v>1</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>1032</v>
-      </c>
       <c r="E80">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F80" t="s">
         <v>17</v>
@@ -5311,7 +5314,7 @@
         <v>90</v>
       </c>
       <c r="E82">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
@@ -5328,7 +5331,7 @@
         <v>93</v>
       </c>
       <c r="E83">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
@@ -5345,7 +5348,7 @@
         <v>910</v>
       </c>
       <c r="E84">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
@@ -5362,7 +5365,7 @@
         <v>911</v>
       </c>
       <c r="E85">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
@@ -5379,7 +5382,7 @@
         <v>95</v>
       </c>
       <c r="E86">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
@@ -5401,39 +5404,39 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B88" t="s">
         <v>1033</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="4">
+        <v>1</v>
+      </c>
+      <c r="D88" s="1" t="s">
         <v>1034</v>
       </c>
-      <c r="C88" s="4">
-        <v>1</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>1035</v>
-      </c>
       <c r="E88">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="B89" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="C89" s="4">
         <v>2</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="E89">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F89" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
@@ -5475,19 +5478,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B92" t="s">
         <v>1064</v>
       </c>
-      <c r="B92" t="s">
-        <v>1065</v>
-      </c>
       <c r="C92" s="4">
         <v>1</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="E92">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
@@ -5521,7 +5524,7 @@
         <v>914</v>
       </c>
       <c r="E94">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F94" t="s">
         <v>488</v>
@@ -5541,7 +5544,7 @@
         <v>915</v>
       </c>
       <c r="E95">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
@@ -5558,7 +5561,7 @@
         <v>916</v>
       </c>
       <c r="E96">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -5575,7 +5578,7 @@
         <v>917</v>
       </c>
       <c r="E97">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
@@ -5592,7 +5595,7 @@
         <v>918</v>
       </c>
       <c r="E98">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F98" t="s">
         <v>135</v>
@@ -5612,7 +5615,7 @@
         <v>919</v>
       </c>
       <c r="E99">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F99" t="s">
         <v>494</v>
@@ -5632,7 +5635,7 @@
         <v>105</v>
       </c>
       <c r="E100">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
@@ -5649,7 +5652,7 @@
         <v>920</v>
       </c>
       <c r="E101">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
@@ -5666,7 +5669,7 @@
         <v>921</v>
       </c>
       <c r="E102">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F102" t="s">
         <v>498</v>
@@ -5723,7 +5726,7 @@
         <v>113</v>
       </c>
       <c r="E105">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F105" t="s">
         <v>110</v>
@@ -5760,7 +5763,7 @@
         <v>923</v>
       </c>
       <c r="E107">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F107" t="s">
         <v>369</v>
@@ -5780,7 +5783,7 @@
         <v>924</v>
       </c>
       <c r="E108">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F108" t="s">
         <v>503</v>
@@ -5800,7 +5803,7 @@
         <v>925</v>
       </c>
       <c r="E109">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
@@ -5817,7 +5820,7 @@
         <v>118</v>
       </c>
       <c r="E110">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
@@ -5834,7 +5837,7 @@
         <v>926</v>
       </c>
       <c r="E111">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
@@ -5851,7 +5854,7 @@
         <v>927</v>
       </c>
       <c r="E112">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F112" t="s">
         <v>507</v>
@@ -5871,7 +5874,7 @@
         <v>121</v>
       </c>
       <c r="E113">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
@@ -5888,7 +5891,7 @@
         <v>123</v>
       </c>
       <c r="E114">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
@@ -5905,7 +5908,7 @@
         <v>1019</v>
       </c>
       <c r="E115">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F115" t="s">
         <v>525</v>
@@ -5925,7 +5928,7 @@
         <v>928</v>
       </c>
       <c r="E116">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F116" t="s">
         <v>529</v>
@@ -5945,7 +5948,7 @@
         <v>929</v>
       </c>
       <c r="E117">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F117" t="s">
         <v>531</v>
@@ -5965,24 +5968,24 @@
         <v>127</v>
       </c>
       <c r="E118">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B119" t="s">
         <v>1066</v>
-      </c>
-      <c r="B119" t="s">
-        <v>1067</v>
       </c>
       <c r="C119" s="4">
         <v>3</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="E119">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -5999,7 +6002,7 @@
         <v>930</v>
       </c>
       <c r="E120">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -6016,7 +6019,7 @@
         <v>127</v>
       </c>
       <c r="E121">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -6033,7 +6036,7 @@
         <v>931</v>
       </c>
       <c r="E122">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
@@ -6050,7 +6053,7 @@
         <v>131</v>
       </c>
       <c r="E123">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F123" t="s">
         <v>132</v>
@@ -6070,7 +6073,7 @@
         <v>138</v>
       </c>
       <c r="E124">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F124" t="s">
         <v>135</v>
@@ -6090,7 +6093,7 @@
         <v>932</v>
       </c>
       <c r="E125">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
@@ -6107,7 +6110,7 @@
         <v>21</v>
       </c>
       <c r="E126">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
@@ -6124,7 +6127,7 @@
         <v>933</v>
       </c>
       <c r="E127">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F127" t="s">
         <v>536</v>
@@ -6144,7 +6147,7 @@
         <v>538</v>
       </c>
       <c r="E128">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
@@ -6161,7 +6164,7 @@
         <v>540</v>
       </c>
       <c r="E129">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
@@ -6178,7 +6181,7 @@
         <v>142</v>
       </c>
       <c r="E130">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
@@ -6195,7 +6198,7 @@
         <v>144</v>
       </c>
       <c r="E131">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F131" t="s">
         <v>631</v>
@@ -6232,7 +6235,7 @@
         <v>551</v>
       </c>
       <c r="E133">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F133" t="s">
         <v>550</v>
@@ -6252,7 +6255,7 @@
         <v>934</v>
       </c>
       <c r="E134">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
@@ -6269,7 +6272,7 @@
         <v>935</v>
       </c>
       <c r="E135">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -6286,7 +6289,7 @@
         <v>151</v>
       </c>
       <c r="E136">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F136" t="s">
         <v>150</v>
@@ -6343,7 +6346,7 @@
         <v>937</v>
       </c>
       <c r="E139">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -6360,7 +6363,7 @@
         <v>559</v>
       </c>
       <c r="E140">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F140" t="s">
         <v>560</v>
@@ -6397,7 +6400,7 @@
         <v>938</v>
       </c>
       <c r="E142">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F142" t="s">
         <v>562</v>
@@ -6417,7 +6420,7 @@
         <v>939</v>
       </c>
       <c r="E143">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F143" t="s">
         <v>564</v>
@@ -6457,7 +6460,7 @@
         <v>940</v>
       </c>
       <c r="E145">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F145" t="s">
         <v>566</v>
@@ -6494,7 +6497,7 @@
         <v>941</v>
       </c>
       <c r="E147">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -6511,7 +6514,7 @@
         <v>942</v>
       </c>
       <c r="E148">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
@@ -6528,7 +6531,7 @@
         <v>943</v>
       </c>
       <c r="E149">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F149" t="s">
         <v>570</v>
@@ -6548,7 +6551,7 @@
         <v>944</v>
       </c>
       <c r="E150">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F150" t="s">
         <v>572</v>
@@ -6556,19 +6559,19 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B151" t="s">
         <v>1036</v>
       </c>
-      <c r="B151" t="s">
+      <c r="C151" s="4">
+        <v>1</v>
+      </c>
+      <c r="D151" s="1" t="s">
         <v>1037</v>
       </c>
-      <c r="C151" s="4">
-        <v>1</v>
-      </c>
-      <c r="D151" s="1" t="s">
-        <v>1038</v>
-      </c>
       <c r="E151">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
@@ -6585,7 +6588,7 @@
         <v>945</v>
       </c>
       <c r="E152">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F152" t="s">
         <v>17</v>
@@ -6593,22 +6596,22 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B153" t="s">
         <v>1070</v>
       </c>
-      <c r="B153" t="s">
+      <c r="C153" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="D153" s="1" t="s">
         <v>1071</v>
       </c>
-      <c r="C153" s="4" t="s">
-        <v>1069</v>
-      </c>
-      <c r="D153" s="1" t="s">
-        <v>1072</v>
-      </c>
       <c r="E153">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F153" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
@@ -6625,7 +6628,7 @@
         <v>946</v>
       </c>
       <c r="E154">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F154" t="s">
         <v>575</v>
@@ -6645,7 +6648,7 @@
         <v>947</v>
       </c>
       <c r="E155">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -6682,7 +6685,7 @@
         <v>168</v>
       </c>
       <c r="E157">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F157" t="s">
         <v>65</v>
@@ -6722,7 +6725,7 @@
         <v>949</v>
       </c>
       <c r="E159">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F159" t="s">
         <v>578</v>
@@ -6759,7 +6762,7 @@
         <v>54</v>
       </c>
       <c r="E161">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
@@ -6810,7 +6813,7 @@
         <v>600</v>
       </c>
       <c r="E164">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
@@ -6861,7 +6864,7 @@
         <v>603</v>
       </c>
       <c r="E167">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F167" t="s">
         <v>604</v>
@@ -6881,7 +6884,7 @@
         <v>179</v>
       </c>
       <c r="E168">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
@@ -6898,7 +6901,7 @@
         <v>953</v>
       </c>
       <c r="E169">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F169" t="s">
         <v>607</v>
@@ -6918,7 +6921,7 @@
         <v>954</v>
       </c>
       <c r="E170">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F170" t="s">
         <v>609</v>
@@ -6926,19 +6929,19 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B171" t="s">
         <v>1081</v>
-      </c>
-      <c r="B171" t="s">
-        <v>1082</v>
       </c>
       <c r="C171" s="4">
         <v>13</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="E171">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
@@ -6972,7 +6975,7 @@
         <v>612</v>
       </c>
       <c r="E173">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F173" t="s">
         <v>613</v>
@@ -6992,7 +6995,7 @@
         <v>186</v>
       </c>
       <c r="E174">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F174" t="s">
         <v>65</v>
@@ -7012,27 +7015,27 @@
         <v>955</v>
       </c>
       <c r="E175">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B176" t="s">
         <v>1077</v>
-      </c>
-      <c r="B176" t="s">
-        <v>1078</v>
       </c>
       <c r="C176" s="4">
         <v>5</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="E176">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F176" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -7049,24 +7052,24 @@
         <v>189</v>
       </c>
       <c r="E177">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B178" t="s">
         <v>1073</v>
-      </c>
-      <c r="B178" t="s">
-        <v>1074</v>
       </c>
       <c r="C178" s="4">
         <v>2</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="E178">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -7083,7 +7086,7 @@
         <v>956</v>
       </c>
       <c r="E179">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
@@ -7100,7 +7103,7 @@
         <v>192</v>
       </c>
       <c r="E180">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F180" t="s">
         <v>17</v>
@@ -7137,7 +7140,7 @@
         <v>957</v>
       </c>
       <c r="E182">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F182" t="s">
         <v>617</v>
@@ -7174,7 +7177,7 @@
         <v>177</v>
       </c>
       <c r="E184">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.2">
@@ -7191,7 +7194,7 @@
         <v>959</v>
       </c>
       <c r="E185">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F185" t="s">
         <v>633</v>
@@ -7199,19 +7202,19 @@
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B186" t="s">
         <v>1083</v>
-      </c>
-      <c r="B186" t="s">
-        <v>1084</v>
       </c>
       <c r="C186" s="4">
         <v>6</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="E186">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.2">
@@ -7233,16 +7236,16 @@
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B188" t="s">
         <v>1039</v>
       </c>
-      <c r="B188" t="s">
+      <c r="C188" s="4">
+        <v>1</v>
+      </c>
+      <c r="D188" s="1" t="s">
         <v>1040</v>
-      </c>
-      <c r="C188" s="4">
-        <v>1</v>
-      </c>
-      <c r="D188" s="1" t="s">
-        <v>1041</v>
       </c>
       <c r="E188">
         <v>14</v>
@@ -7279,7 +7282,7 @@
         <v>113</v>
       </c>
       <c r="E190">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.2">
@@ -7296,7 +7299,7 @@
         <v>202</v>
       </c>
       <c r="E191">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F191" t="s">
         <v>17</v>
@@ -7324,19 +7327,19 @@
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B193" t="s">
+        <v>1087</v>
+      </c>
+      <c r="C193" s="4">
+        <v>1</v>
+      </c>
+      <c r="D193" s="1" t="s">
         <v>1086</v>
       </c>
-      <c r="B193" t="s">
-        <v>1088</v>
-      </c>
-      <c r="C193" s="4">
-        <v>1</v>
-      </c>
-      <c r="D193" s="1" t="s">
-        <v>1087</v>
-      </c>
       <c r="E193">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.2">
@@ -7353,7 +7356,7 @@
         <v>961</v>
       </c>
       <c r="E194">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.2">
@@ -7370,7 +7373,7 @@
         <v>1020</v>
       </c>
       <c r="E195">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F195" t="s">
         <v>647</v>
@@ -7390,24 +7393,24 @@
         <v>649</v>
       </c>
       <c r="E196">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B197" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C197" s="4">
         <v>4</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="E197">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.2">
@@ -7458,7 +7461,7 @@
         <v>208</v>
       </c>
       <c r="E200">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F200" t="s">
         <v>17</v>
@@ -7478,7 +7481,7 @@
         <v>35</v>
       </c>
       <c r="E201">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -7512,7 +7515,7 @@
         <v>964</v>
       </c>
       <c r="E203">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.2">
@@ -7546,7 +7549,7 @@
         <v>217</v>
       </c>
       <c r="E205">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F205" t="s">
         <v>215</v>
@@ -7566,7 +7569,7 @@
         <v>658</v>
       </c>
       <c r="E206">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.2">
@@ -7600,7 +7603,7 @@
         <v>966</v>
       </c>
       <c r="E208">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
@@ -7617,7 +7620,7 @@
         <v>967</v>
       </c>
       <c r="E209">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
@@ -7634,24 +7637,24 @@
         <v>666</v>
       </c>
       <c r="E210">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B211" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="C211" s="4">
         <v>5</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="E211">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
@@ -7673,16 +7676,16 @@
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B213" t="s">
         <v>1095</v>
-      </c>
-      <c r="B213" t="s">
-        <v>1096</v>
       </c>
       <c r="C213" s="4">
         <v>3</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E213">
         <v>11</v>
@@ -7699,13 +7702,10 @@
         <v>1</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>222</v>
+        <v>1117</v>
       </c>
       <c r="E214">
-        <v>11</v>
-      </c>
-      <c r="F214" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
@@ -7739,7 +7739,7 @@
         <v>968</v>
       </c>
       <c r="E216">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F216" t="s">
         <v>668</v>
@@ -7776,7 +7776,7 @@
         <v>189</v>
       </c>
       <c r="E218">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
@@ -7793,7 +7793,7 @@
         <v>234</v>
       </c>
       <c r="E219">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
@@ -7810,7 +7810,7 @@
         <v>177</v>
       </c>
       <c r="E220">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
@@ -7827,7 +7827,7 @@
         <v>969</v>
       </c>
       <c r="E221">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F221" t="s">
         <v>675</v>
@@ -7847,7 +7847,7 @@
         <v>239</v>
       </c>
       <c r="E222">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F222" t="s">
         <v>1024</v>
@@ -7855,22 +7855,22 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B223" t="s">
         <v>1098</v>
-      </c>
-      <c r="B223" t="s">
-        <v>1099</v>
       </c>
       <c r="C223" s="4">
         <v>6</v>
       </c>
       <c r="D223" s="1" t="s">
+        <v>1099</v>
+      </c>
+      <c r="E223">
+        <v>11</v>
+      </c>
+      <c r="F223" t="s">
         <v>1100</v>
-      </c>
-      <c r="E223">
-        <v>10</v>
-      </c>
-      <c r="F223" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
@@ -7887,7 +7887,7 @@
         <v>679</v>
       </c>
       <c r="E224">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F224" t="s">
         <v>680</v>
@@ -7932,16 +7932,16 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
+        <v>1043</v>
+      </c>
+      <c r="B227" t="s">
         <v>1044</v>
       </c>
-      <c r="B227" t="s">
+      <c r="C227" s="4">
+        <v>1</v>
+      </c>
+      <c r="D227" s="1" t="s">
         <v>1045</v>
-      </c>
-      <c r="C227" s="4">
-        <v>1</v>
-      </c>
-      <c r="D227" s="1" t="s">
-        <v>1046</v>
       </c>
       <c r="E227">
         <v>10</v>
@@ -7981,7 +7981,7 @@
         <v>685</v>
       </c>
       <c r="E229">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F229" t="s">
         <v>686</v>
@@ -7989,10 +7989,10 @@
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
+        <v>1041</v>
+      </c>
+      <c r="B230" t="s">
         <v>1042</v>
-      </c>
-      <c r="B230" t="s">
-        <v>1043</v>
       </c>
       <c r="C230" s="4">
         <v>1</v>
@@ -8001,7 +8001,7 @@
         <v>47</v>
       </c>
       <c r="E230">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -8018,7 +8018,7 @@
         <v>245</v>
       </c>
       <c r="E231">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F231" t="s">
         <v>65</v>
@@ -8032,16 +8032,16 @@
         <v>248</v>
       </c>
       <c r="C232" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>247</v>
       </c>
       <c r="E232">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F232" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
@@ -8098,7 +8098,7 @@
         <v>971</v>
       </c>
       <c r="E235">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F235" t="s">
         <v>613</v>
@@ -8138,7 +8138,7 @@
         <v>974</v>
       </c>
       <c r="E237">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F237" t="s">
         <v>699</v>
@@ -8195,7 +8195,7 @@
         <v>260</v>
       </c>
       <c r="E240">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F240" t="s">
         <v>257</v>
@@ -8232,7 +8232,7 @@
         <v>976</v>
       </c>
       <c r="E242">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F242" t="s">
         <v>706</v>
@@ -8252,7 +8252,7 @@
         <v>729</v>
       </c>
       <c r="E243">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F243" t="s">
         <v>730</v>
@@ -8272,7 +8272,7 @@
         <v>977</v>
       </c>
       <c r="E244">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F244" t="s">
         <v>711</v>
@@ -8292,7 +8292,7 @@
         <v>978</v>
       </c>
       <c r="E245">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.2">
@@ -8346,7 +8346,7 @@
         <v>142</v>
       </c>
       <c r="E248">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.2">
@@ -8363,7 +8363,7 @@
         <v>980</v>
       </c>
       <c r="E249">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F249" t="s">
         <v>715</v>
@@ -8403,7 +8403,7 @@
         <v>981</v>
       </c>
       <c r="E251">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.2">
@@ -8420,7 +8420,7 @@
         <v>721</v>
       </c>
       <c r="E252">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F252" t="s">
         <v>613</v>
@@ -8440,7 +8440,7 @@
         <v>266</v>
       </c>
       <c r="E253">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F253" t="s">
         <v>17</v>
@@ -8448,16 +8448,16 @@
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B254" t="s">
         <v>1047</v>
       </c>
-      <c r="B254" t="s">
+      <c r="C254" s="4">
+        <v>1</v>
+      </c>
+      <c r="D254" s="1" t="s">
         <v>1048</v>
-      </c>
-      <c r="C254" s="4">
-        <v>1</v>
-      </c>
-      <c r="D254" s="1" t="s">
-        <v>1049</v>
       </c>
       <c r="E254">
         <v>8</v>
@@ -8477,7 +8477,7 @@
         <v>269</v>
       </c>
       <c r="E255">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.2">
@@ -8534,7 +8534,7 @@
         <v>275</v>
       </c>
       <c r="E258">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F258" t="s">
         <v>17</v>
@@ -8554,7 +8554,7 @@
         <v>278</v>
       </c>
       <c r="E259">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" spans="1:6" x14ac:dyDescent="0.2">
@@ -8571,7 +8571,7 @@
         <v>983</v>
       </c>
       <c r="E260">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F260" t="s">
         <v>730</v>
@@ -8591,7 +8591,7 @@
         <v>984</v>
       </c>
       <c r="E261">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F261" t="s">
         <v>613</v>
@@ -8611,7 +8611,7 @@
         <v>985</v>
       </c>
       <c r="E262">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F262" t="s">
         <v>1025</v>
@@ -8619,39 +8619,39 @@
     </row>
     <row r="263" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B263" t="s">
         <v>1102</v>
       </c>
-      <c r="B263" t="s">
+      <c r="C263" s="4" t="s">
+        <v>1105</v>
+      </c>
+      <c r="D263" s="1" t="s">
         <v>1103</v>
-      </c>
-      <c r="C263" s="4" t="s">
-        <v>1106</v>
-      </c>
-      <c r="D263" s="1" t="s">
-        <v>1104</v>
       </c>
       <c r="E263">
         <v>8</v>
       </c>
       <c r="F263" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="264" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B264" t="s">
         <v>1050</v>
       </c>
-      <c r="B264" t="s">
+      <c r="C264" s="4">
+        <v>1</v>
+      </c>
+      <c r="D264" s="1" t="s">
         <v>1051</v>
       </c>
-      <c r="C264" s="4">
-        <v>1</v>
-      </c>
-      <c r="D264" s="1" t="s">
-        <v>1052</v>
-      </c>
       <c r="E264">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="265" spans="1:6" x14ac:dyDescent="0.2">
@@ -8668,7 +8668,7 @@
         <v>986</v>
       </c>
       <c r="E265">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="266" spans="1:6" x14ac:dyDescent="0.2">
@@ -8722,7 +8722,7 @@
         <v>281</v>
       </c>
       <c r="E268">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="269" spans="1:6" x14ac:dyDescent="0.2">
@@ -8739,7 +8739,7 @@
         <v>284</v>
       </c>
       <c r="E269">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="270" spans="1:6" x14ac:dyDescent="0.2">
@@ -8756,7 +8756,7 @@
         <v>751</v>
       </c>
       <c r="E270">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="271" spans="1:6" x14ac:dyDescent="0.2">
@@ -8773,7 +8773,7 @@
         <v>755</v>
       </c>
       <c r="E271">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="272" spans="1:6" x14ac:dyDescent="0.2">
@@ -8807,7 +8807,7 @@
         <v>989</v>
       </c>
       <c r="E273">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F273" t="s">
         <v>613</v>
@@ -8827,7 +8827,7 @@
         <v>990</v>
       </c>
       <c r="E274">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F274" t="s">
         <v>759</v>
@@ -8847,7 +8847,7 @@
         <v>765</v>
       </c>
       <c r="E275">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F275" t="s">
         <v>766</v>
@@ -8867,7 +8867,7 @@
         <v>991</v>
       </c>
       <c r="E276">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F276" t="s">
         <v>769</v>
@@ -8904,7 +8904,7 @@
         <v>771</v>
       </c>
       <c r="E278">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F278" t="s">
         <v>772</v>
@@ -8941,7 +8941,7 @@
         <v>295</v>
       </c>
       <c r="E280">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="281" spans="1:6" x14ac:dyDescent="0.2">
@@ -8958,7 +8958,7 @@
         <v>992</v>
       </c>
       <c r="E281">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="282" spans="1:6" x14ac:dyDescent="0.2">
@@ -9012,7 +9012,7 @@
         <v>995</v>
       </c>
       <c r="E284">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F284" t="s">
         <v>783</v>
@@ -9032,7 +9032,7 @@
         <v>785</v>
       </c>
       <c r="E285">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F285" t="s">
         <v>786</v>
@@ -9052,7 +9052,7 @@
         <v>996</v>
       </c>
       <c r="E286">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F286" t="s">
         <v>793</v>
@@ -9123,7 +9123,7 @@
         <v>998</v>
       </c>
       <c r="E290">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F290" t="s">
         <v>797</v>
@@ -9143,7 +9143,7 @@
         <v>303</v>
       </c>
       <c r="E291">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F291" t="s">
         <v>65</v>
@@ -9220,7 +9220,7 @@
         <v>823</v>
       </c>
       <c r="E295">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F295" t="s">
         <v>613</v>
@@ -9351,7 +9351,7 @@
         <v>1005</v>
       </c>
       <c r="E302">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F302" t="s">
         <v>820</v>
@@ -9425,7 +9425,7 @@
         <v>1006</v>
       </c>
       <c r="E306">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="307" spans="1:6" x14ac:dyDescent="0.2">
@@ -9638,7 +9638,7 @@
         <v>1011</v>
       </c>
       <c r="E318">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F318" t="s">
         <v>847</v>
@@ -9675,7 +9675,7 @@
         <v>1012</v>
       </c>
       <c r="E320">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F320" t="s">
         <v>849</v>
@@ -9695,7 +9695,7 @@
         <v>335</v>
       </c>
       <c r="E321">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="322" spans="1:6" x14ac:dyDescent="0.2">
@@ -9913,10 +9913,10 @@
     </row>
     <row r="334" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B334" t="s">
         <v>1053</v>
-      </c>
-      <c r="B334" t="s">
-        <v>1054</v>
       </c>
       <c r="C334" s="4">
         <v>1</v>
@@ -10004,259 +10004,260 @@
     <hyperlink ref="D204" r:id="rId69" xr:uid="{7D30DAA1-B71B-1E45-891D-13F493267ADB}"/>
     <hyperlink ref="D205" r:id="rId70" xr:uid="{A7BAD85E-728C-B448-9748-299138DC221D}"/>
     <hyperlink ref="D212" r:id="rId71" xr:uid="{07C10A77-57E3-A640-AF41-7CB5857C68EC}"/>
-    <hyperlink ref="D214" r:id="rId72" xr:uid="{A2AB50DB-6782-DF4C-BAE7-2DCF5644A0D4}"/>
-    <hyperlink ref="D215" r:id="rId73" xr:uid="{7A4F5A51-535D-864F-BAEB-5733166A42C2}"/>
-    <hyperlink ref="D217" r:id="rId74" xr:uid="{20087AD9-B514-4A45-A556-F28E6FB6177E}"/>
-    <hyperlink ref="D218" r:id="rId75" xr:uid="{140B28CA-0F1B-4E49-9252-60FDF2CFEDD2}"/>
-    <hyperlink ref="D219" r:id="rId76" xr:uid="{EF6BD527-CB9D-FA40-8E70-196095151AE3}"/>
-    <hyperlink ref="D220" r:id="rId77" xr:uid="{145B5CD1-EFED-2F43-953B-A7F8A950B266}"/>
-    <hyperlink ref="D222" r:id="rId78" xr:uid="{CC055539-EA65-2A44-AB67-D40081122D0B}"/>
-    <hyperlink ref="D228" r:id="rId79" xr:uid="{29670E32-331F-9F4F-9054-6C2146E9CFAF}"/>
-    <hyperlink ref="D231" r:id="rId80" xr:uid="{3CF381A9-2BED-D14F-B3B3-E8CDD1127E15}"/>
-    <hyperlink ref="D232" r:id="rId81" xr:uid="{46BEEB39-9834-204B-8F42-5E4E02AD1CC8}"/>
-    <hyperlink ref="D233" r:id="rId82" xr:uid="{DF6039C2-942D-F941-B039-6C0585125A48}"/>
-    <hyperlink ref="D238" r:id="rId83" xr:uid="{C36F2CBC-6CED-474D-B943-4EE05D8A68DB}"/>
-    <hyperlink ref="D239" r:id="rId84" xr:uid="{91687819-D39C-354F-BBDD-959D3E40666F}"/>
-    <hyperlink ref="D240" r:id="rId85" xr:uid="{52717691-C640-324C-95B4-F547A03353E8}"/>
-    <hyperlink ref="D246" r:id="rId86" xr:uid="{40BCB520-B32D-1A42-98CC-0707B2D17C55}"/>
-    <hyperlink ref="D248" r:id="rId87" xr:uid="{8D664C2B-4047-8E40-AB59-FB574D27C0F0}"/>
-    <hyperlink ref="D253" r:id="rId88" xr:uid="{A5C7C621-99E8-7E49-BAAF-C487D0B0B6F0}"/>
-    <hyperlink ref="D255" r:id="rId89" xr:uid="{227F77B3-EC11-F94D-8C0A-ADAEB49530FE}"/>
-    <hyperlink ref="D256" r:id="rId90" xr:uid="{5449A3B6-4550-7E45-BFE3-A2151412517D}"/>
-    <hyperlink ref="D258" r:id="rId91" xr:uid="{9B1970C5-93A3-F746-92AB-A89E7E8CF689}"/>
-    <hyperlink ref="D259" r:id="rId92" xr:uid="{761FF4B8-FC0C-0A49-8AC5-D8E1E9282F8B}"/>
-    <hyperlink ref="D268" r:id="rId93" xr:uid="{9349A409-9D9B-F643-AB40-54333637777A}"/>
-    <hyperlink ref="D269" r:id="rId94" xr:uid="{FEE40A4B-E4C8-EC46-84BF-75671911BB09}"/>
-    <hyperlink ref="D272" r:id="rId95" xr:uid="{2C7FFE3C-18CE-2F43-A5B7-CF0F2AD2DA45}"/>
-    <hyperlink ref="D277" r:id="rId96" xr:uid="{177DFCE8-F238-FC48-9435-D1F5FB3E5342}"/>
-    <hyperlink ref="D279" r:id="rId97" xr:uid="{5B9C35DD-B434-734A-8AC0-9FF79409A93E}"/>
-    <hyperlink ref="D280" r:id="rId98" xr:uid="{AD9683CD-DE93-F34B-8D9B-4AECB791ACD7}"/>
-    <hyperlink ref="D287" r:id="rId99" xr:uid="{7D90CA8E-E7E1-A542-B194-CB308F4623B3}"/>
-    <hyperlink ref="D288" r:id="rId100" xr:uid="{6A8B4C79-DD07-2C4F-8129-30870107A3E6}"/>
-    <hyperlink ref="D291" r:id="rId101" xr:uid="{994A7E48-5C46-1F4E-B163-AFBE6FEB2884}"/>
-    <hyperlink ref="D292" r:id="rId102" xr:uid="{F322D0D2-AB44-944E-8B95-963F686507CA}"/>
-    <hyperlink ref="D298" r:id="rId103" xr:uid="{B43E7924-638B-6E4F-A76C-3769082026F5}"/>
-    <hyperlink ref="D301" r:id="rId104" xr:uid="{1AFE93D0-0F38-F047-B526-BAF111BD79B1}"/>
-    <hyperlink ref="D305" r:id="rId105" xr:uid="{22507991-6091-E44E-991C-660BB328BA3F}"/>
-    <hyperlink ref="D307" r:id="rId106" xr:uid="{50D43C9E-4349-0748-AED3-902A699ECD7F}"/>
-    <hyperlink ref="D309" r:id="rId107" xr:uid="{9567162D-DDD6-9A43-A665-14AAFCC19477}"/>
-    <hyperlink ref="D310" r:id="rId108" xr:uid="{66AB3688-4221-C746-BBC0-039CF3B5FEA4}"/>
-    <hyperlink ref="D313" r:id="rId109" xr:uid="{D9F898A2-C89B-7D4F-BBE7-BBCDA1979443}"/>
-    <hyperlink ref="D314" r:id="rId110" xr:uid="{A22A8A7E-BE72-8B44-8C9C-460780EAB097}"/>
-    <hyperlink ref="D316" r:id="rId111" xr:uid="{FD0A4B26-D14E-F04F-B942-FDBBBAC1D9EA}"/>
-    <hyperlink ref="D319" r:id="rId112" xr:uid="{6DCCBC92-ACA2-1848-9087-CBB08E454AB9}"/>
-    <hyperlink ref="D322" r:id="rId113" xr:uid="{C7CCAB57-C8F8-9B40-86F9-315843951AD1}"/>
-    <hyperlink ref="D323" r:id="rId114" xr:uid="{357D3ECE-6992-F745-8118-5E2F2A8418EC}"/>
-    <hyperlink ref="D324" r:id="rId115" xr:uid="{A34D738B-ACFA-5444-82EE-4E7BD3F75DEA}"/>
-    <hyperlink ref="D328" r:id="rId116" xr:uid="{8D514CD8-D64A-C94E-A92D-4D86A95B3C4C}"/>
-    <hyperlink ref="D332" r:id="rId117" xr:uid="{69EB6302-2144-854F-91AA-04F3B786DD8C}"/>
-    <hyperlink ref="D333" r:id="rId118" xr:uid="{AA2367B7-DB8C-AF44-9E54-742F4E0015A9}"/>
-    <hyperlink ref="D8" r:id="rId119" xr:uid="{8B7D21E7-976F-4D4F-95CC-67B93849BE8D}"/>
-    <hyperlink ref="D37" r:id="rId120" xr:uid="{FD2FA91D-7F87-A047-904B-89ABA2F43B35}"/>
-    <hyperlink ref="D115" r:id="rId121" xr:uid="{7A08E6C4-3D98-5348-9C90-9B0AE69E8461}"/>
-    <hyperlink ref="D128" r:id="rId122" xr:uid="{F0978077-8555-FC45-B99A-678BBCF1188E}"/>
-    <hyperlink ref="D129" r:id="rId123" xr:uid="{5EC4CDCC-E050-4547-AD5F-D0903E21043B}"/>
-    <hyperlink ref="D167" r:id="rId124" xr:uid="{2AE285A8-1B62-934B-9C5F-7F730122EB36}"/>
-    <hyperlink ref="D243" r:id="rId125" xr:uid="{4AAE7740-87A2-874A-8D8D-CD24516EAB75}"/>
-    <hyperlink ref="D315" r:id="rId126" xr:uid="{786D22A5-F7E5-7847-AAE7-0FC0FCDFCD7B}"/>
-    <hyperlink ref="D2" r:id="rId127" xr:uid="{E1EC90CB-AAB7-3440-9AE4-53FFFD4EFA9B}"/>
-    <hyperlink ref="D3" r:id="rId128" xr:uid="{52C21954-613C-F04B-9368-1B42E5084F10}"/>
-    <hyperlink ref="D4" r:id="rId129" xr:uid="{291C629C-C068-904F-9373-AC85CF1E73B1}"/>
-    <hyperlink ref="D5" r:id="rId130" xr:uid="{46C742B8-3196-304E-AF8B-7EA0C60E16F1}"/>
-    <hyperlink ref="D6" r:id="rId131" xr:uid="{5F59428A-087C-2C40-A446-9E496536D43D}"/>
-    <hyperlink ref="D9" r:id="rId132" xr:uid="{3EF6AB9B-0B5E-3345-AD51-5B2E4A61811F}"/>
-    <hyperlink ref="D11" r:id="rId133" xr:uid="{5EE585F0-2AA2-FA42-83F8-D9A8B245D508}"/>
-    <hyperlink ref="D12" r:id="rId134" xr:uid="{576FD270-A399-B949-9EE5-5755B03DECFF}"/>
-    <hyperlink ref="D14" r:id="rId135" xr:uid="{99E590A4-EECD-684A-A331-1BB611D91E17}"/>
-    <hyperlink ref="D18" r:id="rId136" xr:uid="{8B4A724F-DB04-374C-80BB-3D986BA1F784}"/>
-    <hyperlink ref="D19" r:id="rId137" xr:uid="{BD844104-B418-9041-A050-08805BC82833}"/>
-    <hyperlink ref="D22" r:id="rId138" xr:uid="{9FF78832-C64A-EB46-A21B-31B6FD5998DB}"/>
-    <hyperlink ref="D23" r:id="rId139" xr:uid="{AFBAF701-7D72-DA49-90F5-FA6B6E3570D4}"/>
-    <hyperlink ref="D24" r:id="rId140" xr:uid="{1C7B1CF9-2D6D-0449-A20B-90EFCC97CC40}"/>
-    <hyperlink ref="D26" r:id="rId141" xr:uid="{3844E160-1EF7-6547-8701-EE943EFF9CC0}"/>
-    <hyperlink ref="D27" r:id="rId142" xr:uid="{63B68F83-0AA0-1844-8D59-CFD45A6ED106}"/>
-    <hyperlink ref="D30" r:id="rId143" xr:uid="{F11D866B-D565-5945-A83D-9155012B17AE}"/>
-    <hyperlink ref="D31" r:id="rId144" xr:uid="{0C442643-BF04-BE45-ADD1-676D02B54AD1}"/>
-    <hyperlink ref="D32" r:id="rId145" xr:uid="{A44AF104-929D-564D-8432-661A2CC654F2}"/>
-    <hyperlink ref="D36" r:id="rId146" xr:uid="{B6E19600-03A4-E842-9AAD-25D618FBA53E}"/>
-    <hyperlink ref="D38" r:id="rId147" xr:uid="{5970DEB3-D7A0-0E44-9ECF-CF85ADAE4A98}"/>
-    <hyperlink ref="D39" r:id="rId148" xr:uid="{DF5AEE36-4DC2-644E-A85E-50193AD9AF82}"/>
-    <hyperlink ref="D41" r:id="rId149" xr:uid="{2F7D4D4B-D5C3-ED43-8E01-E9B098F7B17B}"/>
-    <hyperlink ref="D42" r:id="rId150" xr:uid="{ECD2B11B-BE45-8E41-A986-187578395FE6}"/>
-    <hyperlink ref="D43" r:id="rId151" xr:uid="{F0BB3F6B-EA1E-BC49-802B-EC71FC919DAA}"/>
-    <hyperlink ref="D44" r:id="rId152" xr:uid="{B09BFCEF-AEE2-A449-84C2-609B0CB2027F}"/>
-    <hyperlink ref="D46" r:id="rId153" xr:uid="{7B37C6B6-A58A-BF44-AF24-0191BD555B6B}"/>
-    <hyperlink ref="D48" r:id="rId154" xr:uid="{CF3756F0-1F51-DF4A-8FAD-7625EF1CAA7C}"/>
-    <hyperlink ref="D50" r:id="rId155" xr:uid="{C37CBD8D-504C-D14E-B3D8-45B50EBE479F}"/>
-    <hyperlink ref="D51" r:id="rId156" xr:uid="{2F841105-C353-D94B-9231-290E95F34765}"/>
-    <hyperlink ref="D52" r:id="rId157" xr:uid="{5559D066-48A9-1D4C-9672-C5EBC38AD0A8}"/>
-    <hyperlink ref="D57" r:id="rId158" xr:uid="{F9B9634D-D282-7748-A7C1-A30052C9142A}"/>
-    <hyperlink ref="D58" r:id="rId159" xr:uid="{510591BC-5317-9843-8D7D-4B492540C257}"/>
-    <hyperlink ref="D59" r:id="rId160" xr:uid="{180DA692-7E3A-E448-A5E5-6D979014236D}"/>
-    <hyperlink ref="D61" r:id="rId161" xr:uid="{A0576B82-AB05-BF45-8B1C-740B180E8569}"/>
-    <hyperlink ref="D62" r:id="rId162" xr:uid="{FADF9659-85D3-FD4A-8307-50B6D38AF7FC}"/>
-    <hyperlink ref="D64" r:id="rId163" xr:uid="{F15238AF-7E7F-BC49-9B02-0CE81DB471DD}"/>
-    <hyperlink ref="D66" r:id="rId164" xr:uid="{EDC32405-06B4-C24A-A06D-05D1A82D9AE4}"/>
-    <hyperlink ref="D67" r:id="rId165" xr:uid="{4D334DE7-FA3B-5444-83CD-423AC2E52C1E}"/>
-    <hyperlink ref="D70" r:id="rId166" xr:uid="{8196F7BA-1F29-2B4C-A56D-E1C49C999475}"/>
-    <hyperlink ref="D73" r:id="rId167" xr:uid="{6D37DBB5-2F95-DB41-9E43-A0167C9A377A}"/>
-    <hyperlink ref="D76" r:id="rId168" xr:uid="{4CFCC5C0-E69B-9D4A-A2BF-C21934145FE2}"/>
-    <hyperlink ref="D77" r:id="rId169" xr:uid="{7E943830-22BC-E243-BA8E-DF5B9E31AC84}"/>
-    <hyperlink ref="D79" r:id="rId170" xr:uid="{862BA1FE-673C-6B43-A881-B16F461D9F8B}"/>
-    <hyperlink ref="D81" r:id="rId171" xr:uid="{C06826B8-132E-604D-BEEB-F5F817A79172}"/>
-    <hyperlink ref="D84" r:id="rId172" xr:uid="{36BE41E2-1870-7F41-A5EA-5A0B7E8F6FF4}"/>
-    <hyperlink ref="D85" r:id="rId173" xr:uid="{4FCF6328-AD22-C34F-9FFD-329468E1FE0C}"/>
-    <hyperlink ref="D90" r:id="rId174" xr:uid="{B58C4738-5C7B-F544-8B18-578AE26D3150}"/>
-    <hyperlink ref="D91" r:id="rId175" xr:uid="{121DB5AE-73F5-4542-9191-A7027527830F}"/>
-    <hyperlink ref="D94" r:id="rId176" xr:uid="{0F7FB62A-77D8-464C-B001-D4553C7AC956}"/>
-    <hyperlink ref="D95" r:id="rId177" xr:uid="{6CD623FE-4089-F946-84A3-DD5899C94EBF}"/>
-    <hyperlink ref="D96" r:id="rId178" xr:uid="{C29B4382-6387-B446-BBDC-97823C47F822}"/>
-    <hyperlink ref="D97" r:id="rId179" xr:uid="{37C99FBC-E8FD-BD46-B112-502EAE1EE8A0}"/>
-    <hyperlink ref="D98" r:id="rId180" xr:uid="{15A3E523-44F1-3743-A187-A1C31DDD6829}"/>
-    <hyperlink ref="D99" r:id="rId181" xr:uid="{394E7434-3E97-ED44-B873-015C09391A08}"/>
-    <hyperlink ref="D101" r:id="rId182" xr:uid="{7FF12ADC-06B1-6141-B23F-3577AB8E1061}"/>
-    <hyperlink ref="D102" r:id="rId183" xr:uid="{DFF4AE5E-2E1F-8C47-9717-C87D6D5A2883}"/>
-    <hyperlink ref="D104" r:id="rId184" xr:uid="{2A1B6CD7-4878-B246-945C-87560F305CE1}"/>
-    <hyperlink ref="D107" r:id="rId185" xr:uid="{308C5869-03AC-5446-80CE-3DDA30954279}"/>
-    <hyperlink ref="D108" r:id="rId186" xr:uid="{4186D306-189E-3544-8DB5-E1235CF0998C}"/>
-    <hyperlink ref="D109" r:id="rId187" xr:uid="{294D06E0-AA9A-3F42-9C83-801536D9EB7E}"/>
-    <hyperlink ref="D111" r:id="rId188" xr:uid="{783B5ACF-25C3-6A41-A837-D39AFF74B6F3}"/>
-    <hyperlink ref="D112" r:id="rId189" xr:uid="{F2BEB94C-ED3C-FB41-A9B9-618011223790}"/>
-    <hyperlink ref="D116" r:id="rId190" xr:uid="{199848A5-9FD7-1947-B9FE-2896CA52A9CD}"/>
-    <hyperlink ref="D117" r:id="rId191" xr:uid="{7F2B8DE3-96A7-AB42-B9E3-3405E68A0AEF}"/>
-    <hyperlink ref="D120" r:id="rId192" xr:uid="{EC0E513B-5BA3-AD45-8F90-1C7FDEF84292}"/>
-    <hyperlink ref="D122" r:id="rId193" xr:uid="{7E092351-1D65-584E-943D-87B73F8D1083}"/>
-    <hyperlink ref="D125" r:id="rId194" xr:uid="{41805192-57BA-D745-9825-9E20533445AE}"/>
-    <hyperlink ref="D127" r:id="rId195" xr:uid="{236E0FF1-DBD3-8B44-A2ED-766726AE9A4C}"/>
-    <hyperlink ref="D133" r:id="rId196" xr:uid="{29DD9439-A822-9645-A3D2-7B671DA750CF}"/>
-    <hyperlink ref="D134" r:id="rId197" xr:uid="{C37224D4-66FD-314C-A9E0-996187B8EC40}"/>
-    <hyperlink ref="D135" r:id="rId198" xr:uid="{C4ECA53F-C9DF-094B-9C59-5BA36DF8D21A}"/>
-    <hyperlink ref="D137" r:id="rId199" xr:uid="{F3BE7A2B-25F0-C248-A356-256EBFD6551B}"/>
-    <hyperlink ref="D139" r:id="rId200" xr:uid="{E971C79A-224F-4F45-89DD-ED0D1069A307}"/>
-    <hyperlink ref="D140" r:id="rId201" xr:uid="{DA71B8DD-3CD4-2C40-AEBD-597453A0F967}"/>
-    <hyperlink ref="D142" r:id="rId202" xr:uid="{ACD47C30-2661-BF47-958D-93414F58881D}"/>
-    <hyperlink ref="D143" r:id="rId203" xr:uid="{D2A862E2-A32C-0343-A6BA-5695835D2E76}"/>
-    <hyperlink ref="D145" r:id="rId204" xr:uid="{0634C0CF-A693-D244-8379-7B5236354560}"/>
-    <hyperlink ref="D147" r:id="rId205" xr:uid="{5E421D92-E898-A242-B57F-537FDA339866}"/>
-    <hyperlink ref="D148" r:id="rId206" xr:uid="{E1928FD0-F405-EF42-BF48-252FB13EBF3E}"/>
-    <hyperlink ref="D149" r:id="rId207" xr:uid="{BAF4C302-676C-7943-8158-13A0B83436B3}"/>
-    <hyperlink ref="D150" r:id="rId208" xr:uid="{60585F2B-C3D5-1847-AAE9-035378570CB5}"/>
-    <hyperlink ref="D154" r:id="rId209" xr:uid="{E239B6C9-67FB-DF46-9C05-9AE1818A9730}"/>
-    <hyperlink ref="D155" r:id="rId210" xr:uid="{0C1E1F5B-A0DD-2748-A2DA-243D51626680}"/>
-    <hyperlink ref="D156" r:id="rId211" xr:uid="{0EA8F203-B009-AE45-B052-C0885BE14EC0}"/>
-    <hyperlink ref="D159" r:id="rId212" xr:uid="{5E6F5367-8DA8-CE48-BC50-48B4DE03F331}"/>
-    <hyperlink ref="D160" r:id="rId213" xr:uid="{4FF28A1F-B098-B940-99B3-F069499EE4A2}"/>
-    <hyperlink ref="D162" r:id="rId214" xr:uid="{7179FB86-4642-E941-A5F2-9E680322A323}"/>
-    <hyperlink ref="D163" r:id="rId215" xr:uid="{D1C41524-21C0-0243-BE94-15DF25631EB8}"/>
-    <hyperlink ref="D164" r:id="rId216" xr:uid="{9D0BD335-4E4A-0E43-A765-D13FD1A7D5CE}"/>
-    <hyperlink ref="D166" r:id="rId217" xr:uid="{7F05114F-F931-6143-9BE1-C9CC2BAD3CDE}"/>
-    <hyperlink ref="D169" r:id="rId218" xr:uid="{79644F05-3586-C247-9A43-72FAFF7EADBD}"/>
-    <hyperlink ref="D170" r:id="rId219" xr:uid="{33318DB0-EC47-0347-96C5-5D1DD9857551}"/>
-    <hyperlink ref="D173" r:id="rId220" xr:uid="{32774AD7-7CFB-EC42-BF95-33F8FFA1CE11}"/>
-    <hyperlink ref="D175" r:id="rId221" xr:uid="{B9F8873F-D9C9-324D-BF68-68854FD9FE0F}"/>
-    <hyperlink ref="D179" r:id="rId222" xr:uid="{8465BC4F-BAB4-5F4D-8D65-9058771E8A15}"/>
-    <hyperlink ref="D182" r:id="rId223" xr:uid="{BFF67294-1988-934C-8D94-F154F481B298}"/>
-    <hyperlink ref="D183" r:id="rId224" xr:uid="{30713DB0-23F4-0249-9DE6-B414723AF70F}"/>
-    <hyperlink ref="D185" r:id="rId225" xr:uid="{6A8A41C0-B4F3-4E4F-867D-3F610C17672D}"/>
-    <hyperlink ref="D189" r:id="rId226" xr:uid="{93881ED7-1660-8F4A-BE16-3A52688A4732}"/>
-    <hyperlink ref="D190" r:id="rId227" xr:uid="{EC1C22B1-FBED-3B46-9C14-99277596747A}"/>
-    <hyperlink ref="D192" r:id="rId228" xr:uid="{2A0583F5-E89B-0C4B-ABB8-8C715AA6D644}"/>
-    <hyperlink ref="D195" r:id="rId229" xr:uid="{2A35003C-6807-A94F-ADC8-6F4A871BE0DE}"/>
-    <hyperlink ref="D194" r:id="rId230" xr:uid="{969CFBBB-A52F-4C4C-B65E-9D20FB34E5B7}"/>
-    <hyperlink ref="D196" r:id="rId231" xr:uid="{7EEC399E-D97E-E942-9A7F-16E3BA666380}"/>
-    <hyperlink ref="D198" r:id="rId232" xr:uid="{8C6C3BFD-F48D-3D42-A9FB-EFAC4B25D51A}"/>
-    <hyperlink ref="D202" r:id="rId233" xr:uid="{290E5743-4AF7-624F-95DB-D3BA6DEE692F}"/>
-    <hyperlink ref="D203" r:id="rId234" xr:uid="{F200939D-5882-D74F-BFD9-E1C02BFE57D7}"/>
-    <hyperlink ref="D206" r:id="rId235" xr:uid="{EEC780B1-2542-1F41-B9A0-0043144688E5}"/>
-    <hyperlink ref="D207" r:id="rId236" xr:uid="{D2E6133B-0A97-F646-A602-516415E6C667}"/>
-    <hyperlink ref="D208" r:id="rId237" xr:uid="{AFD38A9D-BCA9-D14C-B0A3-B5A8B164FD8F}"/>
-    <hyperlink ref="D209" r:id="rId238" xr:uid="{6CB54F8E-0E32-DF4B-9792-DC52BAF4A9BF}"/>
-    <hyperlink ref="D210" r:id="rId239" xr:uid="{83F1281A-BB47-A841-8B5D-ABF7A5C6C23C}"/>
-    <hyperlink ref="D216" r:id="rId240" xr:uid="{3EBCA580-4014-FE44-A5E1-8CC779B21626}"/>
-    <hyperlink ref="D221" r:id="rId241" xr:uid="{D8C677F9-36D8-F841-AFAF-6BFDB8D42A48}"/>
-    <hyperlink ref="D224" r:id="rId242" xr:uid="{FE8059BA-72D9-FC43-A4FE-DE894DD51905}"/>
-    <hyperlink ref="D225" r:id="rId243" xr:uid="{1ED7131B-E4EF-144F-A65B-6B4813903681}"/>
-    <hyperlink ref="D226" r:id="rId244" xr:uid="{BDB09020-16F0-C548-BF02-6E0D47A8B509}"/>
-    <hyperlink ref="D229" r:id="rId245" xr:uid="{0ECC7CA5-761D-D44D-8427-43A9AB7FF75E}"/>
-    <hyperlink ref="D235" r:id="rId246" xr:uid="{F70EF9A7-B667-5142-82B0-E1698C8B07E4}"/>
-    <hyperlink ref="D234" r:id="rId247" xr:uid="{0C44F3D3-0F77-3F4F-9DA3-673608C14757}"/>
-    <hyperlink ref="D236" r:id="rId248" xr:uid="{AB68B81D-FB10-4D4D-B52F-D32A32F92D85}"/>
-    <hyperlink ref="D237" r:id="rId249" xr:uid="{63CD33D4-55B1-7445-9DA2-CE9DC29B9A7A}"/>
-    <hyperlink ref="D241" r:id="rId250" xr:uid="{E43FBB97-D54E-744D-93DF-882E46D2B8C6}"/>
-    <hyperlink ref="D242" r:id="rId251" xr:uid="{0CA848E8-8262-0F4E-AA94-7A04D58655FF}"/>
-    <hyperlink ref="D244" r:id="rId252" xr:uid="{60EF7D4C-92B9-4B41-BBD7-D9DF3C646448}"/>
-    <hyperlink ref="D245" r:id="rId253" xr:uid="{D8C98462-B731-B041-8DD2-A361CD6941E1}"/>
-    <hyperlink ref="D247" r:id="rId254" xr:uid="{909D62FB-D7A0-324B-BC45-0DA15CED8789}"/>
-    <hyperlink ref="D249" r:id="rId255" xr:uid="{8CF5D932-8BA6-5A41-8302-7AAABA20957A}"/>
-    <hyperlink ref="D251" r:id="rId256" xr:uid="{1C958DD0-3B00-AC4F-B50D-8C37C5A31569}"/>
-    <hyperlink ref="D252" r:id="rId257" xr:uid="{9FC34C6E-61FF-7E4F-9086-98B1AA608F90}"/>
-    <hyperlink ref="D250" r:id="rId258" xr:uid="{DEFEC865-5E2F-494E-B409-EDD2E9182CFC}"/>
-    <hyperlink ref="D257" r:id="rId259" xr:uid="{2A06F8A2-C724-7C4D-9219-51388A54B795}"/>
-    <hyperlink ref="D260" r:id="rId260" xr:uid="{15E040C0-75BC-814E-9B21-7C18F066FE49}"/>
-    <hyperlink ref="D261" r:id="rId261" xr:uid="{F6A7C7C5-4BB2-C946-B80A-6C905025605E}"/>
-    <hyperlink ref="D262" r:id="rId262" xr:uid="{CC230F8A-63FD-9E4C-B293-79E78C6A2530}"/>
-    <hyperlink ref="D265" r:id="rId263" xr:uid="{A52EEF71-FBD1-304B-A888-D14E0843CF85}"/>
-    <hyperlink ref="D266" r:id="rId264" xr:uid="{7ECA1E78-AD74-3D4C-A369-89B26ECF8BBF}"/>
-    <hyperlink ref="D267" r:id="rId265" xr:uid="{CEE90642-5656-9D47-9CA9-8233907C3D02}"/>
-    <hyperlink ref="D270" r:id="rId266" xr:uid="{3D2BCDA9-8CD3-5B40-905F-D353860859F4}"/>
-    <hyperlink ref="D271" r:id="rId267" xr:uid="{5349A06F-CDFF-ED4B-B030-F6658418C6E7}"/>
-    <hyperlink ref="D273" r:id="rId268" xr:uid="{0109EB7D-6709-BD40-8C66-F6F7162C9767}"/>
-    <hyperlink ref="D274" r:id="rId269" xr:uid="{8BC81ECC-BD46-5A47-8218-88277800DC7A}"/>
-    <hyperlink ref="D275" r:id="rId270" xr:uid="{EA71FBE6-B8F6-2045-98FD-54BC44689C88}"/>
-    <hyperlink ref="D276" r:id="rId271" xr:uid="{9172A930-19AE-3143-918C-1D4FCFD049E9}"/>
-    <hyperlink ref="D278" r:id="rId272" xr:uid="{A15F482C-B9A8-9245-B7AB-B546A0DFD2C9}"/>
-    <hyperlink ref="D281" r:id="rId273" xr:uid="{9244A73B-11B3-F041-ADD2-3A6A9273AE85}"/>
-    <hyperlink ref="D282" r:id="rId274" xr:uid="{C67B31FA-841C-C344-9EAC-4B9EDA0764EF}"/>
-    <hyperlink ref="D283" r:id="rId275" xr:uid="{37729878-7797-FB4C-AB40-0E95AE8B147F}"/>
-    <hyperlink ref="D284" r:id="rId276" xr:uid="{54E57834-F67F-7648-A3D1-D3773CBF39DA}"/>
-    <hyperlink ref="D285" r:id="rId277" xr:uid="{5963250A-E8ED-EF49-8254-9755E0CCD71B}"/>
-    <hyperlink ref="D286" r:id="rId278" xr:uid="{BA9BDB16-CB1F-9E48-A0EE-DA8743CE0081}"/>
-    <hyperlink ref="D289" r:id="rId279" xr:uid="{0554D873-4941-2A46-8D52-BE10419E0F28}"/>
-    <hyperlink ref="D290" r:id="rId280" xr:uid="{01386E23-819D-E345-BA35-119A1A25C2A0}"/>
-    <hyperlink ref="D293" r:id="rId281" xr:uid="{25171CE2-1CB2-6946-9A75-3F3E7ED44C05}"/>
-    <hyperlink ref="D295" r:id="rId282" xr:uid="{7ADB0023-CA4D-8541-B339-2315767931B2}"/>
-    <hyperlink ref="D294" r:id="rId283" xr:uid="{96517723-6D5D-734F-9FC5-286A02A56467}"/>
-    <hyperlink ref="D296" r:id="rId284" xr:uid="{98230D59-4DEE-114D-834E-90DF62C44EFF}"/>
-    <hyperlink ref="D297" r:id="rId285" xr:uid="{91ADCCAD-0BB8-AA45-9692-69FFE5530FA9}"/>
-    <hyperlink ref="D299" r:id="rId286" xr:uid="{04283243-271E-B442-A919-04917B626566}"/>
-    <hyperlink ref="D300" r:id="rId287" xr:uid="{7366E693-471F-5E4A-93A2-9B80F854520F}"/>
-    <hyperlink ref="D302" r:id="rId288" xr:uid="{A9B3A5E4-8D7C-8C4E-8119-AF6636FEB664}"/>
-    <hyperlink ref="D303" r:id="rId289" xr:uid="{D464C05D-7512-C84C-B5AF-7BD927EE68F3}"/>
-    <hyperlink ref="D304" r:id="rId290" xr:uid="{CE286B98-03BF-D74F-8747-C0AB2CAC54A8}"/>
-    <hyperlink ref="D306" r:id="rId291" xr:uid="{DC94427A-9CBA-8E49-B787-B35247C617E3}"/>
-    <hyperlink ref="D308" r:id="rId292" xr:uid="{833862C0-3846-5C42-9E1A-4C02B2E704E6}"/>
-    <hyperlink ref="D311" r:id="rId293" xr:uid="{9E15C553-503C-A641-BAE3-6B4372139B80}"/>
-    <hyperlink ref="D312" r:id="rId294" xr:uid="{FAD0D355-D508-CC45-94DE-50F335C8C6CB}"/>
-    <hyperlink ref="D317" r:id="rId295" xr:uid="{280BB979-A421-3E4E-9BC4-F7CAAB0CCAB0}"/>
-    <hyperlink ref="D318" r:id="rId296" xr:uid="{90C811C8-0A4C-0648-90F1-7A8F982D56BF}"/>
-    <hyperlink ref="D320" r:id="rId297" xr:uid="{0F965516-B5CD-784E-B382-AE2646737C00}"/>
-    <hyperlink ref="D321" r:id="rId298" xr:uid="{01FF6481-4CF6-DA45-8E7E-270690692014}"/>
-    <hyperlink ref="D325" r:id="rId299" xr:uid="{F27D5842-8690-A541-8356-9DDBFF3A8175}"/>
-    <hyperlink ref="D326" r:id="rId300" xr:uid="{918EFC8B-6744-734C-8547-11656858E740}"/>
-    <hyperlink ref="D327" r:id="rId301" xr:uid="{3C529A39-12D8-A248-90C4-293943DEEE8A}"/>
-    <hyperlink ref="D329" r:id="rId302" xr:uid="{BBBA967C-0823-CC4E-B2AD-A20A0521711A}"/>
-    <hyperlink ref="D330" r:id="rId303" xr:uid="{F0634782-B384-D448-9862-FA36060CFB6E}"/>
-    <hyperlink ref="D331" r:id="rId304" xr:uid="{C4B70249-F8A2-F54F-B2D0-FC0CECF00A55}"/>
-    <hyperlink ref="D69" r:id="rId305" xr:uid="{AE6A14FA-3291-3E41-AA6A-2FF88F4E505D}"/>
-    <hyperlink ref="D88" r:id="rId306" xr:uid="{F96D9947-6B61-6C40-8A18-5AA416F68343}"/>
-    <hyperlink ref="D188" r:id="rId307" xr:uid="{ABB7A349-D3A5-D54E-A613-8D49AB686423}"/>
-    <hyperlink ref="D334" r:id="rId308" xr:uid="{F491A530-146C-9547-9004-D97AB3C92F42}"/>
-    <hyperlink ref="D65" r:id="rId309" xr:uid="{BDC7EA8A-893F-DB4A-A9C5-B30E4FAB8244}"/>
-    <hyperlink ref="D89" r:id="rId310" xr:uid="{2D9FED6E-E320-4140-807F-5587F7B0E820}"/>
-    <hyperlink ref="D92" r:id="rId311" xr:uid="{81F394EC-49A5-FD45-9EAD-54FFF24FB537}"/>
-    <hyperlink ref="D119" r:id="rId312" xr:uid="{33A62CA1-44AC-D641-9346-1B14705FD76F}"/>
-    <hyperlink ref="D153" r:id="rId313" xr:uid="{DA90EFB6-C7F1-E64E-AD2E-88F7D9DC1124}"/>
-    <hyperlink ref="D178" r:id="rId314" xr:uid="{5CA50632-83FB-A645-B67E-2A7136BDCE8E}"/>
-    <hyperlink ref="D176" r:id="rId315" xr:uid="{5BD74026-41EA-5441-BBA5-A299CB6F08B1}"/>
-    <hyperlink ref="D171" r:id="rId316" xr:uid="{BAD901B0-EADF-4244-B3AC-28FE199E2C56}"/>
-    <hyperlink ref="D186" r:id="rId317" xr:uid="{E6C149F7-EFCE-BB40-ABE4-5E4B71D71E28}"/>
-    <hyperlink ref="D193" r:id="rId318" xr:uid="{F71394F8-DC57-5044-AF03-606B48C9AA15}"/>
-    <hyperlink ref="D197" r:id="rId319" xr:uid="{C7F93D23-44EF-EC40-924C-DDD5787E87FD}"/>
-    <hyperlink ref="D211" r:id="rId320" xr:uid="{F7473245-FB29-DD4D-9C5E-A566AACA3CD8}"/>
-    <hyperlink ref="D213" r:id="rId321" xr:uid="{B8BBA577-6445-DD4F-910A-6659855216E6}"/>
-    <hyperlink ref="D223" r:id="rId322" xr:uid="{49EFCE25-1915-CE47-8968-69DF293F5F1B}"/>
-    <hyperlink ref="D263" r:id="rId323" xr:uid="{7CF033CB-F215-8544-9FAF-AEAC4D1C033F}"/>
-    <hyperlink ref="D16" r:id="rId324" xr:uid="{025B0F96-BCF6-AD42-A9C3-6D2CAE882DB7}"/>
+    <hyperlink ref="D215" r:id="rId72" xr:uid="{7A4F5A51-535D-864F-BAEB-5733166A42C2}"/>
+    <hyperlink ref="D217" r:id="rId73" xr:uid="{20087AD9-B514-4A45-A556-F28E6FB6177E}"/>
+    <hyperlink ref="D218" r:id="rId74" xr:uid="{140B28CA-0F1B-4E49-9252-60FDF2CFEDD2}"/>
+    <hyperlink ref="D219" r:id="rId75" xr:uid="{EF6BD527-CB9D-FA40-8E70-196095151AE3}"/>
+    <hyperlink ref="D220" r:id="rId76" xr:uid="{145B5CD1-EFED-2F43-953B-A7F8A950B266}"/>
+    <hyperlink ref="D222" r:id="rId77" xr:uid="{CC055539-EA65-2A44-AB67-D40081122D0B}"/>
+    <hyperlink ref="D228" r:id="rId78" xr:uid="{29670E32-331F-9F4F-9054-6C2146E9CFAF}"/>
+    <hyperlink ref="D231" r:id="rId79" xr:uid="{3CF381A9-2BED-D14F-B3B3-E8CDD1127E15}"/>
+    <hyperlink ref="D232" r:id="rId80" xr:uid="{46BEEB39-9834-204B-8F42-5E4E02AD1CC8}"/>
+    <hyperlink ref="D233" r:id="rId81" xr:uid="{DF6039C2-942D-F941-B039-6C0585125A48}"/>
+    <hyperlink ref="D238" r:id="rId82" xr:uid="{C36F2CBC-6CED-474D-B943-4EE05D8A68DB}"/>
+    <hyperlink ref="D239" r:id="rId83" xr:uid="{91687819-D39C-354F-BBDD-959D3E40666F}"/>
+    <hyperlink ref="D240" r:id="rId84" xr:uid="{52717691-C640-324C-95B4-F547A03353E8}"/>
+    <hyperlink ref="D246" r:id="rId85" xr:uid="{40BCB520-B32D-1A42-98CC-0707B2D17C55}"/>
+    <hyperlink ref="D248" r:id="rId86" xr:uid="{8D664C2B-4047-8E40-AB59-FB574D27C0F0}"/>
+    <hyperlink ref="D253" r:id="rId87" xr:uid="{A5C7C621-99E8-7E49-BAAF-C487D0B0B6F0}"/>
+    <hyperlink ref="D255" r:id="rId88" xr:uid="{227F77B3-EC11-F94D-8C0A-ADAEB49530FE}"/>
+    <hyperlink ref="D256" r:id="rId89" xr:uid="{5449A3B6-4550-7E45-BFE3-A2151412517D}"/>
+    <hyperlink ref="D258" r:id="rId90" xr:uid="{9B1970C5-93A3-F746-92AB-A89E7E8CF689}"/>
+    <hyperlink ref="D259" r:id="rId91" xr:uid="{761FF4B8-FC0C-0A49-8AC5-D8E1E9282F8B}"/>
+    <hyperlink ref="D268" r:id="rId92" xr:uid="{9349A409-9D9B-F643-AB40-54333637777A}"/>
+    <hyperlink ref="D269" r:id="rId93" xr:uid="{FEE40A4B-E4C8-EC46-84BF-75671911BB09}"/>
+    <hyperlink ref="D272" r:id="rId94" xr:uid="{2C7FFE3C-18CE-2F43-A5B7-CF0F2AD2DA45}"/>
+    <hyperlink ref="D277" r:id="rId95" xr:uid="{177DFCE8-F238-FC48-9435-D1F5FB3E5342}"/>
+    <hyperlink ref="D279" r:id="rId96" xr:uid="{5B9C35DD-B434-734A-8AC0-9FF79409A93E}"/>
+    <hyperlink ref="D280" r:id="rId97" xr:uid="{AD9683CD-DE93-F34B-8D9B-4AECB791ACD7}"/>
+    <hyperlink ref="D287" r:id="rId98" xr:uid="{7D90CA8E-E7E1-A542-B194-CB308F4623B3}"/>
+    <hyperlink ref="D288" r:id="rId99" xr:uid="{6A8B4C79-DD07-2C4F-8129-30870107A3E6}"/>
+    <hyperlink ref="D291" r:id="rId100" xr:uid="{994A7E48-5C46-1F4E-B163-AFBE6FEB2884}"/>
+    <hyperlink ref="D292" r:id="rId101" xr:uid="{F322D0D2-AB44-944E-8B95-963F686507CA}"/>
+    <hyperlink ref="D298" r:id="rId102" xr:uid="{B43E7924-638B-6E4F-A76C-3769082026F5}"/>
+    <hyperlink ref="D301" r:id="rId103" xr:uid="{1AFE93D0-0F38-F047-B526-BAF111BD79B1}"/>
+    <hyperlink ref="D305" r:id="rId104" xr:uid="{22507991-6091-E44E-991C-660BB328BA3F}"/>
+    <hyperlink ref="D307" r:id="rId105" xr:uid="{50D43C9E-4349-0748-AED3-902A699ECD7F}"/>
+    <hyperlink ref="D309" r:id="rId106" xr:uid="{9567162D-DDD6-9A43-A665-14AAFCC19477}"/>
+    <hyperlink ref="D310" r:id="rId107" xr:uid="{66AB3688-4221-C746-BBC0-039CF3B5FEA4}"/>
+    <hyperlink ref="D313" r:id="rId108" xr:uid="{D9F898A2-C89B-7D4F-BBE7-BBCDA1979443}"/>
+    <hyperlink ref="D314" r:id="rId109" xr:uid="{A22A8A7E-BE72-8B44-8C9C-460780EAB097}"/>
+    <hyperlink ref="D316" r:id="rId110" xr:uid="{FD0A4B26-D14E-F04F-B942-FDBBBAC1D9EA}"/>
+    <hyperlink ref="D319" r:id="rId111" xr:uid="{6DCCBC92-ACA2-1848-9087-CBB08E454AB9}"/>
+    <hyperlink ref="D322" r:id="rId112" xr:uid="{C7CCAB57-C8F8-9B40-86F9-315843951AD1}"/>
+    <hyperlink ref="D323" r:id="rId113" xr:uid="{357D3ECE-6992-F745-8118-5E2F2A8418EC}"/>
+    <hyperlink ref="D324" r:id="rId114" xr:uid="{A34D738B-ACFA-5444-82EE-4E7BD3F75DEA}"/>
+    <hyperlink ref="D328" r:id="rId115" xr:uid="{8D514CD8-D64A-C94E-A92D-4D86A95B3C4C}"/>
+    <hyperlink ref="D332" r:id="rId116" xr:uid="{69EB6302-2144-854F-91AA-04F3B786DD8C}"/>
+    <hyperlink ref="D333" r:id="rId117" xr:uid="{AA2367B7-DB8C-AF44-9E54-742F4E0015A9}"/>
+    <hyperlink ref="D8" r:id="rId118" xr:uid="{8B7D21E7-976F-4D4F-95CC-67B93849BE8D}"/>
+    <hyperlink ref="D37" r:id="rId119" xr:uid="{FD2FA91D-7F87-A047-904B-89ABA2F43B35}"/>
+    <hyperlink ref="D115" r:id="rId120" xr:uid="{7A08E6C4-3D98-5348-9C90-9B0AE69E8461}"/>
+    <hyperlink ref="D128" r:id="rId121" xr:uid="{F0978077-8555-FC45-B99A-678BBCF1188E}"/>
+    <hyperlink ref="D129" r:id="rId122" xr:uid="{5EC4CDCC-E050-4547-AD5F-D0903E21043B}"/>
+    <hyperlink ref="D167" r:id="rId123" xr:uid="{2AE285A8-1B62-934B-9C5F-7F730122EB36}"/>
+    <hyperlink ref="D243" r:id="rId124" xr:uid="{4AAE7740-87A2-874A-8D8D-CD24516EAB75}"/>
+    <hyperlink ref="D315" r:id="rId125" xr:uid="{786D22A5-F7E5-7847-AAE7-0FC0FCDFCD7B}"/>
+    <hyperlink ref="D2" r:id="rId126" xr:uid="{E1EC90CB-AAB7-3440-9AE4-53FFFD4EFA9B}"/>
+    <hyperlink ref="D3" r:id="rId127" xr:uid="{52C21954-613C-F04B-9368-1B42E5084F10}"/>
+    <hyperlink ref="D4" r:id="rId128" xr:uid="{291C629C-C068-904F-9373-AC85CF1E73B1}"/>
+    <hyperlink ref="D5" r:id="rId129" xr:uid="{46C742B8-3196-304E-AF8B-7EA0C60E16F1}"/>
+    <hyperlink ref="D6" r:id="rId130" xr:uid="{5F59428A-087C-2C40-A446-9E496536D43D}"/>
+    <hyperlink ref="D9" r:id="rId131" xr:uid="{3EF6AB9B-0B5E-3345-AD51-5B2E4A61811F}"/>
+    <hyperlink ref="D11" r:id="rId132" xr:uid="{5EE585F0-2AA2-FA42-83F8-D9A8B245D508}"/>
+    <hyperlink ref="D12" r:id="rId133" xr:uid="{576FD270-A399-B949-9EE5-5755B03DECFF}"/>
+    <hyperlink ref="D14" r:id="rId134" xr:uid="{99E590A4-EECD-684A-A331-1BB611D91E17}"/>
+    <hyperlink ref="D18" r:id="rId135" xr:uid="{8B4A724F-DB04-374C-80BB-3D986BA1F784}"/>
+    <hyperlink ref="D19" r:id="rId136" xr:uid="{BD844104-B418-9041-A050-08805BC82833}"/>
+    <hyperlink ref="D22" r:id="rId137" xr:uid="{9FF78832-C64A-EB46-A21B-31B6FD5998DB}"/>
+    <hyperlink ref="D23" r:id="rId138" xr:uid="{AFBAF701-7D72-DA49-90F5-FA6B6E3570D4}"/>
+    <hyperlink ref="D24" r:id="rId139" xr:uid="{1C7B1CF9-2D6D-0449-A20B-90EFCC97CC40}"/>
+    <hyperlink ref="D26" r:id="rId140" xr:uid="{3844E160-1EF7-6547-8701-EE943EFF9CC0}"/>
+    <hyperlink ref="D27" r:id="rId141" xr:uid="{63B68F83-0AA0-1844-8D59-CFD45A6ED106}"/>
+    <hyperlink ref="D30" r:id="rId142" xr:uid="{F11D866B-D565-5945-A83D-9155012B17AE}"/>
+    <hyperlink ref="D31" r:id="rId143" xr:uid="{0C442643-BF04-BE45-ADD1-676D02B54AD1}"/>
+    <hyperlink ref="D32" r:id="rId144" xr:uid="{A44AF104-929D-564D-8432-661A2CC654F2}"/>
+    <hyperlink ref="D36" r:id="rId145" xr:uid="{B6E19600-03A4-E842-9AAD-25D618FBA53E}"/>
+    <hyperlink ref="D38" r:id="rId146" xr:uid="{5970DEB3-D7A0-0E44-9ECF-CF85ADAE4A98}"/>
+    <hyperlink ref="D39" r:id="rId147" xr:uid="{DF5AEE36-4DC2-644E-A85E-50193AD9AF82}"/>
+    <hyperlink ref="D41" r:id="rId148" xr:uid="{2F7D4D4B-D5C3-ED43-8E01-E9B098F7B17B}"/>
+    <hyperlink ref="D42" r:id="rId149" xr:uid="{ECD2B11B-BE45-8E41-A986-187578395FE6}"/>
+    <hyperlink ref="D43" r:id="rId150" xr:uid="{F0BB3F6B-EA1E-BC49-802B-EC71FC919DAA}"/>
+    <hyperlink ref="D44" r:id="rId151" xr:uid="{B09BFCEF-AEE2-A449-84C2-609B0CB2027F}"/>
+    <hyperlink ref="D46" r:id="rId152" xr:uid="{7B37C6B6-A58A-BF44-AF24-0191BD555B6B}"/>
+    <hyperlink ref="D48" r:id="rId153" xr:uid="{CF3756F0-1F51-DF4A-8FAD-7625EF1CAA7C}"/>
+    <hyperlink ref="D50" r:id="rId154" xr:uid="{C37CBD8D-504C-D14E-B3D8-45B50EBE479F}"/>
+    <hyperlink ref="D51" r:id="rId155" xr:uid="{2F841105-C353-D94B-9231-290E95F34765}"/>
+    <hyperlink ref="D52" r:id="rId156" xr:uid="{5559D066-48A9-1D4C-9672-C5EBC38AD0A8}"/>
+    <hyperlink ref="D57" r:id="rId157" xr:uid="{F9B9634D-D282-7748-A7C1-A30052C9142A}"/>
+    <hyperlink ref="D58" r:id="rId158" xr:uid="{510591BC-5317-9843-8D7D-4B492540C257}"/>
+    <hyperlink ref="D59" r:id="rId159" xr:uid="{180DA692-7E3A-E448-A5E5-6D979014236D}"/>
+    <hyperlink ref="D61" r:id="rId160" xr:uid="{A0576B82-AB05-BF45-8B1C-740B180E8569}"/>
+    <hyperlink ref="D62" r:id="rId161" xr:uid="{FADF9659-85D3-FD4A-8307-50B6D38AF7FC}"/>
+    <hyperlink ref="D64" r:id="rId162" xr:uid="{F15238AF-7E7F-BC49-9B02-0CE81DB471DD}"/>
+    <hyperlink ref="D66" r:id="rId163" xr:uid="{EDC32405-06B4-C24A-A06D-05D1A82D9AE4}"/>
+    <hyperlink ref="D67" r:id="rId164" xr:uid="{4D334DE7-FA3B-5444-83CD-423AC2E52C1E}"/>
+    <hyperlink ref="D70" r:id="rId165" xr:uid="{8196F7BA-1F29-2B4C-A56D-E1C49C999475}"/>
+    <hyperlink ref="D73" r:id="rId166" xr:uid="{6D37DBB5-2F95-DB41-9E43-A0167C9A377A}"/>
+    <hyperlink ref="D76" r:id="rId167" xr:uid="{4CFCC5C0-E69B-9D4A-A2BF-C21934145FE2}"/>
+    <hyperlink ref="D77" r:id="rId168" xr:uid="{7E943830-22BC-E243-BA8E-DF5B9E31AC84}"/>
+    <hyperlink ref="D79" r:id="rId169" xr:uid="{862BA1FE-673C-6B43-A881-B16F461D9F8B}"/>
+    <hyperlink ref="D81" r:id="rId170" xr:uid="{C06826B8-132E-604D-BEEB-F5F817A79172}"/>
+    <hyperlink ref="D84" r:id="rId171" xr:uid="{36BE41E2-1870-7F41-A5EA-5A0B7E8F6FF4}"/>
+    <hyperlink ref="D85" r:id="rId172" xr:uid="{4FCF6328-AD22-C34F-9FFD-329468E1FE0C}"/>
+    <hyperlink ref="D90" r:id="rId173" xr:uid="{B58C4738-5C7B-F544-8B18-578AE26D3150}"/>
+    <hyperlink ref="D91" r:id="rId174" xr:uid="{121DB5AE-73F5-4542-9191-A7027527830F}"/>
+    <hyperlink ref="D94" r:id="rId175" xr:uid="{0F7FB62A-77D8-464C-B001-D4553C7AC956}"/>
+    <hyperlink ref="D95" r:id="rId176" xr:uid="{6CD623FE-4089-F946-84A3-DD5899C94EBF}"/>
+    <hyperlink ref="D96" r:id="rId177" xr:uid="{C29B4382-6387-B446-BBDC-97823C47F822}"/>
+    <hyperlink ref="D97" r:id="rId178" xr:uid="{37C99FBC-E8FD-BD46-B112-502EAE1EE8A0}"/>
+    <hyperlink ref="D98" r:id="rId179" xr:uid="{15A3E523-44F1-3743-A187-A1C31DDD6829}"/>
+    <hyperlink ref="D99" r:id="rId180" xr:uid="{394E7434-3E97-ED44-B873-015C09391A08}"/>
+    <hyperlink ref="D101" r:id="rId181" xr:uid="{7FF12ADC-06B1-6141-B23F-3577AB8E1061}"/>
+    <hyperlink ref="D102" r:id="rId182" xr:uid="{DFF4AE5E-2E1F-8C47-9717-C87D6D5A2883}"/>
+    <hyperlink ref="D104" r:id="rId183" xr:uid="{2A1B6CD7-4878-B246-945C-87560F305CE1}"/>
+    <hyperlink ref="D107" r:id="rId184" xr:uid="{308C5869-03AC-5446-80CE-3DDA30954279}"/>
+    <hyperlink ref="D108" r:id="rId185" xr:uid="{4186D306-189E-3544-8DB5-E1235CF0998C}"/>
+    <hyperlink ref="D109" r:id="rId186" xr:uid="{294D06E0-AA9A-3F42-9C83-801536D9EB7E}"/>
+    <hyperlink ref="D111" r:id="rId187" xr:uid="{783B5ACF-25C3-6A41-A837-D39AFF74B6F3}"/>
+    <hyperlink ref="D112" r:id="rId188" xr:uid="{F2BEB94C-ED3C-FB41-A9B9-618011223790}"/>
+    <hyperlink ref="D116" r:id="rId189" xr:uid="{199848A5-9FD7-1947-B9FE-2896CA52A9CD}"/>
+    <hyperlink ref="D117" r:id="rId190" xr:uid="{7F2B8DE3-96A7-AB42-B9E3-3405E68A0AEF}"/>
+    <hyperlink ref="D120" r:id="rId191" xr:uid="{EC0E513B-5BA3-AD45-8F90-1C7FDEF84292}"/>
+    <hyperlink ref="D122" r:id="rId192" xr:uid="{7E092351-1D65-584E-943D-87B73F8D1083}"/>
+    <hyperlink ref="D125" r:id="rId193" xr:uid="{41805192-57BA-D745-9825-9E20533445AE}"/>
+    <hyperlink ref="D127" r:id="rId194" xr:uid="{236E0FF1-DBD3-8B44-A2ED-766726AE9A4C}"/>
+    <hyperlink ref="D133" r:id="rId195" xr:uid="{29DD9439-A822-9645-A3D2-7B671DA750CF}"/>
+    <hyperlink ref="D134" r:id="rId196" xr:uid="{C37224D4-66FD-314C-A9E0-996187B8EC40}"/>
+    <hyperlink ref="D135" r:id="rId197" xr:uid="{C4ECA53F-C9DF-094B-9C59-5BA36DF8D21A}"/>
+    <hyperlink ref="D137" r:id="rId198" xr:uid="{F3BE7A2B-25F0-C248-A356-256EBFD6551B}"/>
+    <hyperlink ref="D139" r:id="rId199" xr:uid="{E971C79A-224F-4F45-89DD-ED0D1069A307}"/>
+    <hyperlink ref="D140" r:id="rId200" xr:uid="{DA71B8DD-3CD4-2C40-AEBD-597453A0F967}"/>
+    <hyperlink ref="D142" r:id="rId201" xr:uid="{ACD47C30-2661-BF47-958D-93414F58881D}"/>
+    <hyperlink ref="D143" r:id="rId202" xr:uid="{D2A862E2-A32C-0343-A6BA-5695835D2E76}"/>
+    <hyperlink ref="D145" r:id="rId203" xr:uid="{0634C0CF-A693-D244-8379-7B5236354560}"/>
+    <hyperlink ref="D147" r:id="rId204" xr:uid="{5E421D92-E898-A242-B57F-537FDA339866}"/>
+    <hyperlink ref="D148" r:id="rId205" xr:uid="{E1928FD0-F405-EF42-BF48-252FB13EBF3E}"/>
+    <hyperlink ref="D149" r:id="rId206" xr:uid="{BAF4C302-676C-7943-8158-13A0B83436B3}"/>
+    <hyperlink ref="D150" r:id="rId207" xr:uid="{60585F2B-C3D5-1847-AAE9-035378570CB5}"/>
+    <hyperlink ref="D154" r:id="rId208" xr:uid="{E239B6C9-67FB-DF46-9C05-9AE1818A9730}"/>
+    <hyperlink ref="D155" r:id="rId209" xr:uid="{0C1E1F5B-A0DD-2748-A2DA-243D51626680}"/>
+    <hyperlink ref="D156" r:id="rId210" xr:uid="{0EA8F203-B009-AE45-B052-C0885BE14EC0}"/>
+    <hyperlink ref="D159" r:id="rId211" xr:uid="{5E6F5367-8DA8-CE48-BC50-48B4DE03F331}"/>
+    <hyperlink ref="D160" r:id="rId212" xr:uid="{4FF28A1F-B098-B940-99B3-F069499EE4A2}"/>
+    <hyperlink ref="D162" r:id="rId213" xr:uid="{7179FB86-4642-E941-A5F2-9E680322A323}"/>
+    <hyperlink ref="D163" r:id="rId214" xr:uid="{D1C41524-21C0-0243-BE94-15DF25631EB8}"/>
+    <hyperlink ref="D164" r:id="rId215" xr:uid="{9D0BD335-4E4A-0E43-A765-D13FD1A7D5CE}"/>
+    <hyperlink ref="D166" r:id="rId216" xr:uid="{7F05114F-F931-6143-9BE1-C9CC2BAD3CDE}"/>
+    <hyperlink ref="D169" r:id="rId217" xr:uid="{79644F05-3586-C247-9A43-72FAFF7EADBD}"/>
+    <hyperlink ref="D170" r:id="rId218" xr:uid="{33318DB0-EC47-0347-96C5-5D1DD9857551}"/>
+    <hyperlink ref="D173" r:id="rId219" xr:uid="{32774AD7-7CFB-EC42-BF95-33F8FFA1CE11}"/>
+    <hyperlink ref="D175" r:id="rId220" xr:uid="{B9F8873F-D9C9-324D-BF68-68854FD9FE0F}"/>
+    <hyperlink ref="D179" r:id="rId221" xr:uid="{8465BC4F-BAB4-5F4D-8D65-9058771E8A15}"/>
+    <hyperlink ref="D182" r:id="rId222" xr:uid="{BFF67294-1988-934C-8D94-F154F481B298}"/>
+    <hyperlink ref="D183" r:id="rId223" xr:uid="{30713DB0-23F4-0249-9DE6-B414723AF70F}"/>
+    <hyperlink ref="D185" r:id="rId224" xr:uid="{6A8A41C0-B4F3-4E4F-867D-3F610C17672D}"/>
+    <hyperlink ref="D189" r:id="rId225" xr:uid="{93881ED7-1660-8F4A-BE16-3A52688A4732}"/>
+    <hyperlink ref="D190" r:id="rId226" xr:uid="{EC1C22B1-FBED-3B46-9C14-99277596747A}"/>
+    <hyperlink ref="D192" r:id="rId227" xr:uid="{2A0583F5-E89B-0C4B-ABB8-8C715AA6D644}"/>
+    <hyperlink ref="D195" r:id="rId228" xr:uid="{2A35003C-6807-A94F-ADC8-6F4A871BE0DE}"/>
+    <hyperlink ref="D194" r:id="rId229" xr:uid="{969CFBBB-A52F-4C4C-B65E-9D20FB34E5B7}"/>
+    <hyperlink ref="D196" r:id="rId230" xr:uid="{7EEC399E-D97E-E942-9A7F-16E3BA666380}"/>
+    <hyperlink ref="D198" r:id="rId231" xr:uid="{8C6C3BFD-F48D-3D42-A9FB-EFAC4B25D51A}"/>
+    <hyperlink ref="D202" r:id="rId232" xr:uid="{290E5743-4AF7-624F-95DB-D3BA6DEE692F}"/>
+    <hyperlink ref="D203" r:id="rId233" xr:uid="{F200939D-5882-D74F-BFD9-E1C02BFE57D7}"/>
+    <hyperlink ref="D206" r:id="rId234" xr:uid="{EEC780B1-2542-1F41-B9A0-0043144688E5}"/>
+    <hyperlink ref="D207" r:id="rId235" xr:uid="{D2E6133B-0A97-F646-A602-516415E6C667}"/>
+    <hyperlink ref="D208" r:id="rId236" xr:uid="{AFD38A9D-BCA9-D14C-B0A3-B5A8B164FD8F}"/>
+    <hyperlink ref="D209" r:id="rId237" xr:uid="{6CB54F8E-0E32-DF4B-9792-DC52BAF4A9BF}"/>
+    <hyperlink ref="D210" r:id="rId238" xr:uid="{83F1281A-BB47-A841-8B5D-ABF7A5C6C23C}"/>
+    <hyperlink ref="D216" r:id="rId239" xr:uid="{3EBCA580-4014-FE44-A5E1-8CC779B21626}"/>
+    <hyperlink ref="D221" r:id="rId240" xr:uid="{D8C677F9-36D8-F841-AFAF-6BFDB8D42A48}"/>
+    <hyperlink ref="D224" r:id="rId241" xr:uid="{FE8059BA-72D9-FC43-A4FE-DE894DD51905}"/>
+    <hyperlink ref="D225" r:id="rId242" xr:uid="{1ED7131B-E4EF-144F-A65B-6B4813903681}"/>
+    <hyperlink ref="D226" r:id="rId243" xr:uid="{BDB09020-16F0-C548-BF02-6E0D47A8B509}"/>
+    <hyperlink ref="D229" r:id="rId244" xr:uid="{0ECC7CA5-761D-D44D-8427-43A9AB7FF75E}"/>
+    <hyperlink ref="D235" r:id="rId245" xr:uid="{F70EF9A7-B667-5142-82B0-E1698C8B07E4}"/>
+    <hyperlink ref="D234" r:id="rId246" xr:uid="{0C44F3D3-0F77-3F4F-9DA3-673608C14757}"/>
+    <hyperlink ref="D236" r:id="rId247" xr:uid="{AB68B81D-FB10-4D4D-B52F-D32A32F92D85}"/>
+    <hyperlink ref="D237" r:id="rId248" xr:uid="{63CD33D4-55B1-7445-9DA2-CE9DC29B9A7A}"/>
+    <hyperlink ref="D241" r:id="rId249" xr:uid="{E43FBB97-D54E-744D-93DF-882E46D2B8C6}"/>
+    <hyperlink ref="D242" r:id="rId250" xr:uid="{0CA848E8-8262-0F4E-AA94-7A04D58655FF}"/>
+    <hyperlink ref="D244" r:id="rId251" xr:uid="{60EF7D4C-92B9-4B41-BBD7-D9DF3C646448}"/>
+    <hyperlink ref="D245" r:id="rId252" xr:uid="{D8C98462-B731-B041-8DD2-A361CD6941E1}"/>
+    <hyperlink ref="D247" r:id="rId253" xr:uid="{909D62FB-D7A0-324B-BC45-0DA15CED8789}"/>
+    <hyperlink ref="D249" r:id="rId254" xr:uid="{8CF5D932-8BA6-5A41-8302-7AAABA20957A}"/>
+    <hyperlink ref="D251" r:id="rId255" xr:uid="{1C958DD0-3B00-AC4F-B50D-8C37C5A31569}"/>
+    <hyperlink ref="D252" r:id="rId256" xr:uid="{9FC34C6E-61FF-7E4F-9086-98B1AA608F90}"/>
+    <hyperlink ref="D250" r:id="rId257" xr:uid="{DEFEC865-5E2F-494E-B409-EDD2E9182CFC}"/>
+    <hyperlink ref="D257" r:id="rId258" xr:uid="{2A06F8A2-C724-7C4D-9219-51388A54B795}"/>
+    <hyperlink ref="D260" r:id="rId259" xr:uid="{15E040C0-75BC-814E-9B21-7C18F066FE49}"/>
+    <hyperlink ref="D261" r:id="rId260" xr:uid="{F6A7C7C5-4BB2-C946-B80A-6C905025605E}"/>
+    <hyperlink ref="D262" r:id="rId261" xr:uid="{CC230F8A-63FD-9E4C-B293-79E78C6A2530}"/>
+    <hyperlink ref="D265" r:id="rId262" xr:uid="{A52EEF71-FBD1-304B-A888-D14E0843CF85}"/>
+    <hyperlink ref="D266" r:id="rId263" xr:uid="{7ECA1E78-AD74-3D4C-A369-89B26ECF8BBF}"/>
+    <hyperlink ref="D267" r:id="rId264" xr:uid="{CEE90642-5656-9D47-9CA9-8233907C3D02}"/>
+    <hyperlink ref="D270" r:id="rId265" xr:uid="{3D2BCDA9-8CD3-5B40-905F-D353860859F4}"/>
+    <hyperlink ref="D271" r:id="rId266" xr:uid="{5349A06F-CDFF-ED4B-B030-F6658418C6E7}"/>
+    <hyperlink ref="D273" r:id="rId267" xr:uid="{0109EB7D-6709-BD40-8C66-F6F7162C9767}"/>
+    <hyperlink ref="D274" r:id="rId268" xr:uid="{8BC81ECC-BD46-5A47-8218-88277800DC7A}"/>
+    <hyperlink ref="D275" r:id="rId269" xr:uid="{EA71FBE6-B8F6-2045-98FD-54BC44689C88}"/>
+    <hyperlink ref="D276" r:id="rId270" xr:uid="{9172A930-19AE-3143-918C-1D4FCFD049E9}"/>
+    <hyperlink ref="D278" r:id="rId271" xr:uid="{A15F482C-B9A8-9245-B7AB-B546A0DFD2C9}"/>
+    <hyperlink ref="D281" r:id="rId272" xr:uid="{9244A73B-11B3-F041-ADD2-3A6A9273AE85}"/>
+    <hyperlink ref="D282" r:id="rId273" xr:uid="{C67B31FA-841C-C344-9EAC-4B9EDA0764EF}"/>
+    <hyperlink ref="D283" r:id="rId274" xr:uid="{37729878-7797-FB4C-AB40-0E95AE8B147F}"/>
+    <hyperlink ref="D284" r:id="rId275" xr:uid="{54E57834-F67F-7648-A3D1-D3773CBF39DA}"/>
+    <hyperlink ref="D285" r:id="rId276" xr:uid="{5963250A-E8ED-EF49-8254-9755E0CCD71B}"/>
+    <hyperlink ref="D286" r:id="rId277" xr:uid="{BA9BDB16-CB1F-9E48-A0EE-DA8743CE0081}"/>
+    <hyperlink ref="D289" r:id="rId278" xr:uid="{0554D873-4941-2A46-8D52-BE10419E0F28}"/>
+    <hyperlink ref="D290" r:id="rId279" xr:uid="{01386E23-819D-E345-BA35-119A1A25C2A0}"/>
+    <hyperlink ref="D293" r:id="rId280" xr:uid="{25171CE2-1CB2-6946-9A75-3F3E7ED44C05}"/>
+    <hyperlink ref="D295" r:id="rId281" xr:uid="{7ADB0023-CA4D-8541-B339-2315767931B2}"/>
+    <hyperlink ref="D294" r:id="rId282" xr:uid="{96517723-6D5D-734F-9FC5-286A02A56467}"/>
+    <hyperlink ref="D296" r:id="rId283" xr:uid="{98230D59-4DEE-114D-834E-90DF62C44EFF}"/>
+    <hyperlink ref="D297" r:id="rId284" xr:uid="{91ADCCAD-0BB8-AA45-9692-69FFE5530FA9}"/>
+    <hyperlink ref="D299" r:id="rId285" xr:uid="{04283243-271E-B442-A919-04917B626566}"/>
+    <hyperlink ref="D300" r:id="rId286" xr:uid="{7366E693-471F-5E4A-93A2-9B80F854520F}"/>
+    <hyperlink ref="D302" r:id="rId287" xr:uid="{A9B3A5E4-8D7C-8C4E-8119-AF6636FEB664}"/>
+    <hyperlink ref="D303" r:id="rId288" xr:uid="{D464C05D-7512-C84C-B5AF-7BD927EE68F3}"/>
+    <hyperlink ref="D304" r:id="rId289" xr:uid="{CE286B98-03BF-D74F-8747-C0AB2CAC54A8}"/>
+    <hyperlink ref="D306" r:id="rId290" xr:uid="{DC94427A-9CBA-8E49-B787-B35247C617E3}"/>
+    <hyperlink ref="D308" r:id="rId291" xr:uid="{833862C0-3846-5C42-9E1A-4C02B2E704E6}"/>
+    <hyperlink ref="D311" r:id="rId292" xr:uid="{9E15C553-503C-A641-BAE3-6B4372139B80}"/>
+    <hyperlink ref="D312" r:id="rId293" xr:uid="{FAD0D355-D508-CC45-94DE-50F335C8C6CB}"/>
+    <hyperlink ref="D317" r:id="rId294" xr:uid="{280BB979-A421-3E4E-9BC4-F7CAAB0CCAB0}"/>
+    <hyperlink ref="D318" r:id="rId295" xr:uid="{90C811C8-0A4C-0648-90F1-7A8F982D56BF}"/>
+    <hyperlink ref="D320" r:id="rId296" xr:uid="{0F965516-B5CD-784E-B382-AE2646737C00}"/>
+    <hyperlink ref="D321" r:id="rId297" xr:uid="{01FF6481-4CF6-DA45-8E7E-270690692014}"/>
+    <hyperlink ref="D325" r:id="rId298" xr:uid="{F27D5842-8690-A541-8356-9DDBFF3A8175}"/>
+    <hyperlink ref="D326" r:id="rId299" xr:uid="{918EFC8B-6744-734C-8547-11656858E740}"/>
+    <hyperlink ref="D327" r:id="rId300" xr:uid="{3C529A39-12D8-A248-90C4-293943DEEE8A}"/>
+    <hyperlink ref="D329" r:id="rId301" xr:uid="{BBBA967C-0823-CC4E-B2AD-A20A0521711A}"/>
+    <hyperlink ref="D330" r:id="rId302" xr:uid="{F0634782-B384-D448-9862-FA36060CFB6E}"/>
+    <hyperlink ref="D331" r:id="rId303" xr:uid="{C4B70249-F8A2-F54F-B2D0-FC0CECF00A55}"/>
+    <hyperlink ref="D69" r:id="rId304" xr:uid="{AE6A14FA-3291-3E41-AA6A-2FF88F4E505D}"/>
+    <hyperlink ref="D88" r:id="rId305" xr:uid="{F96D9947-6B61-6C40-8A18-5AA416F68343}"/>
+    <hyperlink ref="D188" r:id="rId306" xr:uid="{ABB7A349-D3A5-D54E-A613-8D49AB686423}"/>
+    <hyperlink ref="D334" r:id="rId307" xr:uid="{F491A530-146C-9547-9004-D97AB3C92F42}"/>
+    <hyperlink ref="D65" r:id="rId308" xr:uid="{BDC7EA8A-893F-DB4A-A9C5-B30E4FAB8244}"/>
+    <hyperlink ref="D89" r:id="rId309" xr:uid="{2D9FED6E-E320-4140-807F-5587F7B0E820}"/>
+    <hyperlink ref="D92" r:id="rId310" xr:uid="{81F394EC-49A5-FD45-9EAD-54FFF24FB537}"/>
+    <hyperlink ref="D119" r:id="rId311" xr:uid="{33A62CA1-44AC-D641-9346-1B14705FD76F}"/>
+    <hyperlink ref="D153" r:id="rId312" xr:uid="{DA90EFB6-C7F1-E64E-AD2E-88F7D9DC1124}"/>
+    <hyperlink ref="D178" r:id="rId313" xr:uid="{5CA50632-83FB-A645-B67E-2A7136BDCE8E}"/>
+    <hyperlink ref="D176" r:id="rId314" xr:uid="{5BD74026-41EA-5441-BBA5-A299CB6F08B1}"/>
+    <hyperlink ref="D171" r:id="rId315" xr:uid="{BAD901B0-EADF-4244-B3AC-28FE199E2C56}"/>
+    <hyperlink ref="D186" r:id="rId316" xr:uid="{E6C149F7-EFCE-BB40-ABE4-5E4B71D71E28}"/>
+    <hyperlink ref="D193" r:id="rId317" xr:uid="{F71394F8-DC57-5044-AF03-606B48C9AA15}"/>
+    <hyperlink ref="D197" r:id="rId318" xr:uid="{C7F93D23-44EF-EC40-924C-DDD5787E87FD}"/>
+    <hyperlink ref="D211" r:id="rId319" xr:uid="{F7473245-FB29-DD4D-9C5E-A566AACA3CD8}"/>
+    <hyperlink ref="D213" r:id="rId320" xr:uid="{B8BBA577-6445-DD4F-910A-6659855216E6}"/>
+    <hyperlink ref="D223" r:id="rId321" xr:uid="{49EFCE25-1915-CE47-8968-69DF293F5F1B}"/>
+    <hyperlink ref="D263" r:id="rId322" xr:uid="{7CF033CB-F215-8544-9FAF-AEAC4D1C033F}"/>
+    <hyperlink ref="D16" r:id="rId323" xr:uid="{025B0F96-BCF6-AD42-A9C3-6D2CAE882DB7}"/>
+    <hyperlink ref="D214" r:id="rId324" xr:uid="{A2AB50DB-6782-DF4C-BAE7-2DCF5644A0D4}"/>
+    <hyperlink ref="D227" r:id="rId325" xr:uid="{A310A7CD-57CC-6342-BFD5-D4F9248051D7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Latest as of minor revision round
</commit_message>
<xml_diff>
--- a/Supplementary_materials/Supplementary Table 2.xlsx
+++ b/Supplementary_materials/Supplementary Table 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simonguo/myDocuments/git_local_repo/COVIDnetwork/Supplementary_materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D78F79A-9C5B-4249-AAA5-EAC721C98B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56186B12-9E36-A340-BEA6-6D30052C8DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{2EE752A0-736C-C649-8CDE-11D356C6D5DD}"/>
   </bookViews>
@@ -2394,9 +2394,6 @@
     <t>Number of hits matched to COVID-19 (as of Dec27 2020, * means additional comments about number of hits)</t>
   </si>
   <si>
-    <t>Number of connections to 57 SARS-Cov-2 interacting human proteins</t>
-  </si>
-  <si>
     <t>https://pubmed.ncbi.nlm.nih.gov/34162861/</t>
   </si>
   <si>
@@ -3112,6 +3109,9 @@
   </si>
   <si>
     <t>APLN APEL</t>
+  </si>
+  <si>
+    <t>Number of connections to experimentally validated nodes</t>
   </si>
 </sst>
 </file>
@@ -3488,7 +3488,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H287" sqref="H287"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3512,7 +3512,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>785</v>
+        <v>1024</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>483</v>
@@ -3523,7 +3523,7 @@
         <v>222</v>
       </c>
       <c r="B2" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -3540,7 +3540,7 @@
         <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3560,7 +3560,7 @@
         <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -3620,7 +3620,7 @@
         <v>232</v>
       </c>
       <c r="B7" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C7">
         <v>7</v>
@@ -3640,7 +3640,7 @@
         <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -3677,7 +3677,7 @@
         <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C10">
         <v>37</v>
@@ -3694,7 +3694,7 @@
         <v>263</v>
       </c>
       <c r="B11" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -3731,7 +3731,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3748,7 +3748,7 @@
         <v>226</v>
       </c>
       <c r="B14" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C14">
         <v>8</v>
@@ -3785,7 +3785,7 @@
         <v>229</v>
       </c>
       <c r="B16" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C16" t="s">
         <v>237</v>
@@ -3805,7 +3805,7 @@
         <v>225</v>
       </c>
       <c r="B17" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -3839,7 +3839,7 @@
         <v>257</v>
       </c>
       <c r="B19" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C19">
         <v>7</v>
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -3893,7 +3893,7 @@
         <v>258</v>
       </c>
       <c r="B22" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -3913,7 +3913,7 @@
         <v>253</v>
       </c>
       <c r="B23" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -3930,7 +3930,7 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -3950,7 +3950,7 @@
         <v>281</v>
       </c>
       <c r="B25" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -3967,7 +3967,7 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -4004,7 +4004,7 @@
         <v>280</v>
       </c>
       <c r="B28" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -4024,7 +4024,7 @@
         <v>73</v>
       </c>
       <c r="B29" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -4041,7 +4041,7 @@
         <v>243</v>
       </c>
       <c r="B30" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C30">
         <v>2</v>
@@ -4058,7 +4058,7 @@
         <v>244</v>
       </c>
       <c r="B31" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -4078,7 +4078,7 @@
         <v>262</v>
       </c>
       <c r="B32" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C32">
         <v>2</v>
@@ -4095,7 +4095,7 @@
         <v>246</v>
       </c>
       <c r="B33" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -4115,7 +4115,7 @@
         <v>58</v>
       </c>
       <c r="B34" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -4132,7 +4132,7 @@
         <v>261</v>
       </c>
       <c r="B35" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -4149,7 +4149,7 @@
         <v>311</v>
       </c>
       <c r="B36" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C36">
         <v>2</v>
@@ -4166,7 +4166,7 @@
         <v>254</v>
       </c>
       <c r="B37" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C37" t="s">
         <v>255</v>
@@ -4186,7 +4186,7 @@
         <v>274</v>
       </c>
       <c r="B38" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -4203,7 +4203,7 @@
         <v>328</v>
       </c>
       <c r="B39" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C39" t="s">
         <v>329</v>
@@ -4243,7 +4243,7 @@
         <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C41">
         <v>16</v>
@@ -4317,7 +4317,7 @@
         <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -4334,7 +4334,7 @@
         <v>248</v>
       </c>
       <c r="B46" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C46">
         <v>3</v>
@@ -4368,7 +4368,7 @@
         <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -4385,7 +4385,7 @@
         <v>45</v>
       </c>
       <c r="B49" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C49">
         <v>1</v>
@@ -4402,7 +4402,7 @@
         <v>334</v>
       </c>
       <c r="B50" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C50">
         <v>10</v>
@@ -4419,7 +4419,7 @@
         <v>13</v>
       </c>
       <c r="B51" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C51">
         <v>1</v>
@@ -4476,7 +4476,7 @@
         <v>24</v>
       </c>
       <c r="B54" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -4493,7 +4493,7 @@
         <v>268</v>
       </c>
       <c r="B55" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -4510,7 +4510,7 @@
         <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -4530,7 +4530,7 @@
         <v>269</v>
       </c>
       <c r="B57" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -4570,7 +4570,7 @@
         <v>66</v>
       </c>
       <c r="B59" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -4587,7 +4587,7 @@
         <v>65</v>
       </c>
       <c r="B60" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -4604,7 +4604,7 @@
         <v>267</v>
       </c>
       <c r="B61" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -4641,7 +4641,7 @@
         <v>370</v>
       </c>
       <c r="B63" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C63">
         <v>7</v>
@@ -4658,7 +4658,7 @@
         <v>27</v>
       </c>
       <c r="B64" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -4695,7 +4695,7 @@
         <v>39</v>
       </c>
       <c r="B66" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -4712,7 +4712,7 @@
         <v>293</v>
       </c>
       <c r="B67" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -4729,7 +4729,7 @@
         <v>294</v>
       </c>
       <c r="B68" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C68">
         <v>6</v>
@@ -4749,7 +4749,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C69">
         <v>1</v>
@@ -4766,7 +4766,7 @@
         <v>318</v>
       </c>
       <c r="B70" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C70">
         <v>9</v>
@@ -4786,7 +4786,7 @@
         <v>41</v>
       </c>
       <c r="B71" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C71">
         <v>1</v>
@@ -4806,7 +4806,7 @@
         <v>317</v>
       </c>
       <c r="B72" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -4826,7 +4826,7 @@
         <v>86</v>
       </c>
       <c r="B73" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C73">
         <v>1</v>
@@ -4843,7 +4843,7 @@
         <v>272</v>
       </c>
       <c r="B74" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -4883,7 +4883,7 @@
         <v>282</v>
       </c>
       <c r="B76" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -4900,7 +4900,7 @@
         <v>283</v>
       </c>
       <c r="B77" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C77">
         <v>4</v>
@@ -4940,7 +4940,7 @@
         <v>321</v>
       </c>
       <c r="B79" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C79">
         <v>2</v>
@@ -4957,7 +4957,7 @@
         <v>331</v>
       </c>
       <c r="B80" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C80">
         <v>2</v>
@@ -4977,7 +4977,7 @@
         <v>76</v>
       </c>
       <c r="B81" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C81">
         <v>1</v>
@@ -4994,7 +4994,7 @@
         <v>292</v>
       </c>
       <c r="B82" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C82">
         <v>3</v>
@@ -5011,7 +5011,7 @@
         <v>742</v>
       </c>
       <c r="B83" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C83">
         <v>1</v>
@@ -5048,7 +5048,7 @@
         <v>55</v>
       </c>
       <c r="B85" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C85">
         <v>1</v>
@@ -5068,7 +5068,7 @@
         <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -5085,7 +5085,7 @@
         <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C87">
         <v>1</v>
@@ -5102,7 +5102,7 @@
         <v>379</v>
       </c>
       <c r="B88" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -5119,7 +5119,7 @@
         <v>306</v>
       </c>
       <c r="B89" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C89">
         <v>4</v>
@@ -5173,7 +5173,7 @@
         <v>307</v>
       </c>
       <c r="B92" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C92">
         <v>9</v>
@@ -5190,7 +5190,7 @@
         <v>80</v>
       </c>
       <c r="B93" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C93">
         <v>1</v>
@@ -5207,7 +5207,7 @@
         <v>337</v>
       </c>
       <c r="B94" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C94">
         <v>4</v>
@@ -5224,7 +5224,7 @@
         <v>346</v>
       </c>
       <c r="B95" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C95">
         <v>7</v>
@@ -5258,7 +5258,7 @@
         <v>357</v>
       </c>
       <c r="B97" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C97">
         <v>6</v>
@@ -5278,7 +5278,7 @@
         <v>362</v>
       </c>
       <c r="B98" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C98">
         <v>11</v>
@@ -5295,7 +5295,7 @@
         <v>422</v>
       </c>
       <c r="B99" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C99">
         <v>3</v>
@@ -5312,7 +5312,7 @@
         <v>713</v>
       </c>
       <c r="B100" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -5329,7 +5329,7 @@
         <v>715</v>
       </c>
       <c r="B101" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C101">
         <v>1</v>
@@ -5349,7 +5349,7 @@
         <v>71</v>
       </c>
       <c r="B102" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -5366,7 +5366,7 @@
         <v>326</v>
       </c>
       <c r="B103" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C103">
         <v>11</v>
@@ -5386,7 +5386,7 @@
         <v>320</v>
       </c>
       <c r="B104" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C104">
         <v>2</v>
@@ -5403,7 +5403,7 @@
         <v>84</v>
       </c>
       <c r="B105" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C105">
         <v>1</v>
@@ -5420,7 +5420,7 @@
         <v>333</v>
       </c>
       <c r="B106" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C106">
         <v>2</v>
@@ -5474,7 +5474,7 @@
         <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C109">
         <v>1</v>
@@ -5491,7 +5491,7 @@
         <v>351</v>
       </c>
       <c r="B110" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C110" t="s">
         <v>352</v>
@@ -5511,7 +5511,7 @@
         <v>363</v>
       </c>
       <c r="B111" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C111">
         <v>5</v>
@@ -5531,7 +5531,7 @@
         <v>371</v>
       </c>
       <c r="B112" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C112">
         <v>20</v>
@@ -5591,7 +5591,7 @@
         <v>739</v>
       </c>
       <c r="B115" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C115">
         <v>2</v>
@@ -5611,7 +5611,7 @@
         <v>377</v>
       </c>
       <c r="B116" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -5628,7 +5628,7 @@
         <v>308</v>
       </c>
       <c r="B117" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C117">
         <v>2</v>
@@ -5645,7 +5645,7 @@
         <v>315</v>
       </c>
       <c r="B118" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -5665,7 +5665,7 @@
         <v>365</v>
       </c>
       <c r="B119" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C119">
         <v>24</v>
@@ -5685,7 +5685,7 @@
         <v>124</v>
       </c>
       <c r="B120" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -5702,7 +5702,7 @@
         <v>42</v>
       </c>
       <c r="B121" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C121">
         <v>1</v>
@@ -5719,7 +5719,7 @@
         <v>717</v>
       </c>
       <c r="B122" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C122">
         <v>1</v>
@@ -5736,7 +5736,7 @@
         <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C123">
         <v>1</v>
@@ -5790,7 +5790,7 @@
         <v>285</v>
       </c>
       <c r="B126" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C126" t="s">
         <v>286</v>
@@ -5810,7 +5810,7 @@
         <v>387</v>
       </c>
       <c r="B127" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C127" t="s">
         <v>388</v>
@@ -5830,7 +5830,7 @@
         <v>390</v>
       </c>
       <c r="B128" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C128">
         <v>7</v>
@@ -5850,7 +5850,7 @@
         <v>82</v>
       </c>
       <c r="B129" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C129">
         <v>1</v>
@@ -5867,7 +5867,7 @@
         <v>343</v>
       </c>
       <c r="B130" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C130">
         <v>18</v>
@@ -5887,7 +5887,7 @@
         <v>403</v>
       </c>
       <c r="B131" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C131">
         <v>6</v>
@@ -5904,7 +5904,7 @@
         <v>456</v>
       </c>
       <c r="B132" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C132">
         <v>3</v>
@@ -5924,7 +5924,7 @@
         <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C133">
         <v>1</v>
@@ -5964,7 +5964,7 @@
         <v>398</v>
       </c>
       <c r="B135" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C135">
         <v>3</v>
@@ -5984,7 +5984,7 @@
         <v>404</v>
       </c>
       <c r="B136" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C136">
         <v>1</v>
@@ -6004,7 +6004,7 @@
         <v>355</v>
       </c>
       <c r="B137" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C137">
         <v>156</v>
@@ -6024,7 +6024,7 @@
         <v>367</v>
       </c>
       <c r="B138" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C138" t="s">
         <v>368</v>
@@ -6061,7 +6061,7 @@
         <v>90</v>
       </c>
       <c r="B140" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C140">
         <v>1</v>
@@ -6078,7 +6078,7 @@
         <v>105</v>
       </c>
       <c r="B141" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C141">
         <v>1</v>
@@ -6095,7 +6095,7 @@
         <v>119</v>
       </c>
       <c r="B142" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -6115,7 +6115,7 @@
         <v>120</v>
       </c>
       <c r="B143" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C143">
         <v>1</v>
@@ -6149,7 +6149,7 @@
         <v>60</v>
       </c>
       <c r="B145" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C145">
         <v>1</v>
@@ -6166,7 +6166,7 @@
         <v>322</v>
       </c>
       <c r="B146" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C146">
         <v>7</v>
@@ -6203,7 +6203,7 @@
         <v>383</v>
       </c>
       <c r="B148" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C148">
         <v>2</v>
@@ -6237,7 +6237,7 @@
         <v>410</v>
       </c>
       <c r="B150" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C150">
         <v>3</v>
@@ -6274,7 +6274,7 @@
         <v>350</v>
       </c>
       <c r="B152" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C152">
         <v>6</v>
@@ -6291,7 +6291,7 @@
         <v>92</v>
       </c>
       <c r="B153" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C153">
         <v>1</v>
@@ -6308,7 +6308,7 @@
         <v>99</v>
       </c>
       <c r="B154" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C154">
         <v>1</v>
@@ -6348,7 +6348,7 @@
         <v>384</v>
       </c>
       <c r="B156" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C156">
         <v>2</v>
@@ -6368,7 +6368,7 @@
         <v>392</v>
       </c>
       <c r="B157" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C157" t="s">
         <v>393</v>
@@ -6405,7 +6405,7 @@
         <v>98</v>
       </c>
       <c r="B159" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C159">
         <v>1</v>
@@ -6439,7 +6439,7 @@
         <v>415</v>
       </c>
       <c r="B161" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C161">
         <v>16</v>
@@ -6459,7 +6459,7 @@
         <v>765</v>
       </c>
       <c r="B162" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C162">
         <v>3</v>
@@ -6476,7 +6476,7 @@
         <v>111</v>
       </c>
       <c r="B163" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C163">
         <v>1</v>
@@ -6493,7 +6493,7 @@
         <v>763</v>
       </c>
       <c r="B164" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C164">
         <v>5</v>
@@ -6510,7 +6510,7 @@
         <v>519</v>
       </c>
       <c r="B165" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C165">
         <v>1</v>
@@ -6530,7 +6530,7 @@
         <v>104</v>
       </c>
       <c r="B166" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C166">
         <v>1</v>
@@ -6570,7 +6570,7 @@
         <v>309</v>
       </c>
       <c r="B168" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C168">
         <v>25</v>
@@ -6590,7 +6590,7 @@
         <v>95</v>
       </c>
       <c r="B169" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C169">
         <v>1</v>
@@ -6610,7 +6610,7 @@
         <v>757</v>
       </c>
       <c r="B170" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C170">
         <v>6</v>
@@ -6627,7 +6627,7 @@
         <v>131</v>
       </c>
       <c r="B171" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C171">
         <v>1</v>
@@ -6644,7 +6644,7 @@
         <v>426</v>
       </c>
       <c r="B172" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C172">
         <v>2</v>
@@ -6661,7 +6661,7 @@
         <v>159</v>
       </c>
       <c r="B173" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C173">
         <v>1</v>
@@ -6729,7 +6729,7 @@
         <v>419</v>
       </c>
       <c r="B177" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C177">
         <v>8</v>
@@ -6746,7 +6746,7 @@
         <v>133</v>
       </c>
       <c r="B178" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C178">
         <v>1</v>
@@ -6763,13 +6763,13 @@
         <v>137</v>
       </c>
       <c r="B179" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C179">
         <v>1</v>
       </c>
       <c r="D179" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="E179">
         <v>45</v>
@@ -6780,7 +6780,7 @@
         <v>417</v>
       </c>
       <c r="B180" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -6797,7 +6797,7 @@
         <v>761</v>
       </c>
       <c r="B181" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C181">
         <v>4</v>
@@ -6814,7 +6814,7 @@
         <v>427</v>
       </c>
       <c r="B182" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C182">
         <v>2</v>
@@ -6831,7 +6831,7 @@
         <v>428</v>
       </c>
       <c r="B183" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C183">
         <v>5</v>
@@ -6848,7 +6848,7 @@
         <v>135</v>
       </c>
       <c r="B184" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C184">
         <v>1</v>
@@ -6882,7 +6882,7 @@
         <v>491</v>
       </c>
       <c r="B186" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C186">
         <v>1</v>
@@ -6899,7 +6899,7 @@
         <v>499</v>
       </c>
       <c r="B187" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C187" t="s">
         <v>500</v>
@@ -6919,7 +6919,7 @@
         <v>107</v>
       </c>
       <c r="B188" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="C188">
         <v>1</v>
@@ -6953,7 +6953,7 @@
         <v>126</v>
       </c>
       <c r="B190" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C190">
         <v>1</v>
@@ -6973,7 +6973,7 @@
         <v>128</v>
       </c>
       <c r="B191" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C191">
         <v>1</v>
@@ -6990,7 +6990,7 @@
         <v>423</v>
       </c>
       <c r="B192" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C192">
         <v>2</v>
@@ -7007,7 +7007,7 @@
         <v>767</v>
       </c>
       <c r="B193" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C193">
         <v>6</v>
@@ -7027,7 +7027,7 @@
         <v>725</v>
       </c>
       <c r="B194" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C194">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>397</v>
       </c>
       <c r="B197" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="C197">
         <v>3</v>
@@ -7115,7 +7115,7 @@
         <v>429</v>
       </c>
       <c r="B199" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C199">
         <v>11</v>
@@ -7132,7 +7132,7 @@
         <v>431</v>
       </c>
       <c r="B200" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="C200">
         <v>4</v>
@@ -7152,7 +7152,7 @@
         <v>141</v>
       </c>
       <c r="B201" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="C201">
         <v>1</v>
@@ -7189,7 +7189,7 @@
         <v>487</v>
       </c>
       <c r="B203" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="C203">
         <v>10</v>
@@ -7209,7 +7209,7 @@
         <v>759</v>
       </c>
       <c r="B204" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="C204">
         <v>1</v>
@@ -7246,7 +7246,7 @@
         <v>167</v>
       </c>
       <c r="B206" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C206">
         <v>1</v>
@@ -7266,7 +7266,7 @@
         <v>510</v>
       </c>
       <c r="B207" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C207" t="s">
         <v>511</v>
@@ -7303,7 +7303,7 @@
         <v>482</v>
       </c>
       <c r="B209" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="C209">
         <v>3</v>
@@ -7320,7 +7320,7 @@
         <v>726</v>
       </c>
       <c r="B210" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="C210">
         <v>1</v>
@@ -7340,7 +7340,7 @@
         <v>449</v>
       </c>
       <c r="B211" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="C211">
         <v>5</v>
@@ -7360,7 +7360,7 @@
         <v>461</v>
       </c>
       <c r="B212" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="C212">
         <v>3</v>
@@ -7417,7 +7417,7 @@
         <v>489</v>
       </c>
       <c r="B215" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="C215">
         <v>1</v>
@@ -7434,7 +7434,7 @@
         <v>524</v>
       </c>
       <c r="B216" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="C216">
         <v>2</v>
@@ -7454,7 +7454,7 @@
         <v>109</v>
       </c>
       <c r="B217" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="C217">
         <v>1</v>
@@ -7471,7 +7471,7 @@
         <v>169</v>
       </c>
       <c r="B218" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="C218">
         <v>1</v>
@@ -7488,7 +7488,7 @@
         <v>462</v>
       </c>
       <c r="B219" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="C219">
         <v>3</v>
@@ -7525,7 +7525,7 @@
         <v>139</v>
       </c>
       <c r="B221" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C221">
         <v>1</v>
@@ -7542,7 +7542,7 @@
         <v>442</v>
       </c>
       <c r="B222" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="C222">
         <v>4</v>
@@ -7562,7 +7562,7 @@
         <v>458</v>
       </c>
       <c r="B223" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="C223" t="s">
         <v>286</v>
@@ -7582,7 +7582,7 @@
         <v>476</v>
       </c>
       <c r="B224" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="C224" t="s">
         <v>286</v>
@@ -7622,7 +7622,7 @@
         <v>176</v>
       </c>
       <c r="B226" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="C226">
         <v>1</v>
@@ -7639,7 +7639,7 @@
         <v>185</v>
       </c>
       <c r="B227" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="C227">
         <v>1</v>
@@ -7656,7 +7656,7 @@
         <v>142</v>
       </c>
       <c r="B228" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="C228">
         <v>1</v>
@@ -7744,7 +7744,7 @@
         <v>174</v>
       </c>
       <c r="B233" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -7761,7 +7761,7 @@
         <v>146</v>
       </c>
       <c r="B234" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="C234">
         <v>1</v>
@@ -7778,7 +7778,7 @@
         <v>151</v>
       </c>
       <c r="B235" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C235">
         <v>1</v>
@@ -7798,7 +7798,7 @@
         <v>467</v>
       </c>
       <c r="B236" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="C236">
         <v>3</v>
@@ -7815,7 +7815,7 @@
         <v>163</v>
       </c>
       <c r="B237" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="C237">
         <v>1</v>
@@ -7832,7 +7832,7 @@
         <v>480</v>
       </c>
       <c r="B238" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C238" t="s">
         <v>255</v>
@@ -7852,7 +7852,7 @@
         <v>731</v>
       </c>
       <c r="B239" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="C239">
         <v>1</v>
@@ -7869,7 +7869,7 @@
         <v>199</v>
       </c>
       <c r="B240" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C240">
         <v>1</v>
@@ -7886,7 +7886,7 @@
         <v>202</v>
       </c>
       <c r="B241" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="C241">
         <v>1</v>
@@ -7903,7 +7903,7 @@
         <v>459</v>
       </c>
       <c r="B242" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="C242">
         <v>45</v>
@@ -7923,7 +7923,7 @@
         <v>158</v>
       </c>
       <c r="B243" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -7960,7 +7960,7 @@
         <v>475</v>
       </c>
       <c r="B245" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="C245" t="s">
         <v>286</v>
@@ -7980,7 +7980,7 @@
         <v>161</v>
       </c>
       <c r="B246" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="C246">
         <v>1</v>
@@ -8000,7 +8000,7 @@
         <v>481</v>
       </c>
       <c r="B247" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C247">
         <v>6</v>
@@ -8037,7 +8037,7 @@
         <v>505</v>
       </c>
       <c r="B249" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="C249">
         <v>1</v>
@@ -8057,7 +8057,7 @@
         <v>157</v>
       </c>
       <c r="B250" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="C250">
         <v>1</v>
@@ -8074,7 +8074,7 @@
         <v>165</v>
       </c>
       <c r="B251" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="C251">
         <v>1</v>
@@ -8094,7 +8094,7 @@
         <v>188</v>
       </c>
       <c r="B252" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="C252">
         <v>1</v>
@@ -8131,7 +8131,7 @@
         <v>521</v>
       </c>
       <c r="B254" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="C254">
         <v>7</v>
@@ -8168,7 +8168,7 @@
         <v>156</v>
       </c>
       <c r="B256" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="C256">
         <v>1</v>
@@ -8188,7 +8188,7 @@
         <v>178</v>
       </c>
       <c r="B257" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="C257">
         <v>1</v>
@@ -8205,7 +8205,7 @@
         <v>545</v>
       </c>
       <c r="B258" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="C258">
         <v>1</v>
@@ -8222,7 +8222,7 @@
         <v>553</v>
       </c>
       <c r="B259" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="C259" t="s">
         <v>554</v>
@@ -8242,7 +8242,7 @@
         <v>733</v>
       </c>
       <c r="B260" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="C260">
         <v>1</v>
@@ -8282,7 +8282,7 @@
         <v>207</v>
       </c>
       <c r="B262" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="C262">
         <v>1</v>
@@ -8299,7 +8299,7 @@
         <v>536</v>
       </c>
       <c r="B263" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C263" t="s">
         <v>537</v>
@@ -8319,7 +8319,7 @@
         <v>453</v>
       </c>
       <c r="B264" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="C264">
         <v>3</v>
@@ -8339,7 +8339,7 @@
         <v>503</v>
       </c>
       <c r="B265" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C265">
         <v>11</v>
@@ -8359,7 +8359,7 @@
         <v>181</v>
       </c>
       <c r="B266" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C266">
         <v>1</v>
@@ -8376,7 +8376,7 @@
         <v>513</v>
       </c>
       <c r="B267" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="C267">
         <v>7</v>
@@ -8396,7 +8396,7 @@
         <v>179</v>
       </c>
       <c r="B268" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C268">
         <v>1</v>
@@ -8413,7 +8413,7 @@
         <v>523</v>
       </c>
       <c r="B269" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C269">
         <v>2</v>
@@ -8430,7 +8430,7 @@
         <v>528</v>
       </c>
       <c r="B270" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C270">
         <v>5</v>
@@ -8450,7 +8450,7 @@
         <v>465</v>
       </c>
       <c r="B271" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C271">
         <v>12</v>
@@ -8470,7 +8470,7 @@
         <v>187</v>
       </c>
       <c r="B272" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="C272">
         <v>1</v>
@@ -8490,7 +8490,7 @@
         <v>526</v>
       </c>
       <c r="B273" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C273">
         <v>9</v>
@@ -8510,7 +8510,7 @@
         <v>532</v>
       </c>
       <c r="B274" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C274" t="s">
         <v>533</v>
@@ -8550,7 +8550,7 @@
         <v>539</v>
       </c>
       <c r="B276" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="C276">
         <v>8</v>
@@ -8570,7 +8570,7 @@
         <v>549</v>
       </c>
       <c r="B277" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="C277">
         <v>8</v>
@@ -8607,7 +8607,7 @@
         <v>534</v>
       </c>
       <c r="B279" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="C279">
         <v>6</v>
@@ -8627,7 +8627,7 @@
         <v>538</v>
       </c>
       <c r="B280" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="C280">
         <v>2</v>
@@ -8644,7 +8644,7 @@
         <v>512</v>
       </c>
       <c r="B281" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="C281">
         <v>2</v>
@@ -8661,7 +8661,7 @@
         <v>530</v>
       </c>
       <c r="B282" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="C282" t="s">
         <v>531</v>
@@ -8681,7 +8681,7 @@
         <v>190</v>
       </c>
       <c r="B283" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="C283">
         <v>1</v>
@@ -8698,7 +8698,7 @@
         <v>192</v>
       </c>
       <c r="B284" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="C284">
         <v>1</v>
@@ -8715,7 +8715,7 @@
         <v>548</v>
       </c>
       <c r="B285" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="C285">
         <v>4</v>
@@ -8732,7 +8732,7 @@
         <v>556</v>
       </c>
       <c r="B286" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="C286">
         <v>7</v>
@@ -8752,7 +8752,7 @@
         <v>211</v>
       </c>
       <c r="B287" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="C287">
         <v>1</v>
@@ -8769,7 +8769,7 @@
         <v>542</v>
       </c>
       <c r="B288" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C288" t="s">
         <v>543</v>
@@ -8789,7 +8789,7 @@
         <v>194</v>
       </c>
       <c r="B289" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="C289">
         <v>1</v>
@@ -8806,7 +8806,7 @@
         <v>551</v>
       </c>
       <c r="B290" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="C290">
         <v>4</v>
@@ -8823,7 +8823,7 @@
         <v>563</v>
       </c>
       <c r="B291" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="C291">
         <v>2</v>
@@ -8840,7 +8840,7 @@
         <v>558</v>
       </c>
       <c r="B292" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="C292">
         <v>2</v>
@@ -8857,7 +8857,7 @@
         <v>196</v>
       </c>
       <c r="B293" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C293">
         <v>1</v>
@@ -8874,7 +8874,7 @@
         <v>197</v>
       </c>
       <c r="B294" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="C294">
         <v>1</v>
@@ -8891,7 +8891,7 @@
         <v>201</v>
       </c>
       <c r="B295" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="C295">
         <v>1</v>
@@ -8911,7 +8911,7 @@
         <v>204</v>
       </c>
       <c r="B296" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="C296">
         <v>1</v>
@@ -8928,7 +8928,7 @@
         <v>552</v>
       </c>
       <c r="B297" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="C297">
         <v>2</v>
@@ -8945,7 +8945,7 @@
         <v>205</v>
       </c>
       <c r="B298" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="C298">
         <v>1</v>
@@ -8962,7 +8962,7 @@
         <v>209</v>
       </c>
       <c r="B299" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C299">
         <v>1</v>
@@ -8982,7 +8982,7 @@
         <v>213</v>
       </c>
       <c r="B300" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="C300">
         <v>1</v>
@@ -9002,7 +9002,7 @@
         <v>559</v>
       </c>
       <c r="B301" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C301">
         <v>2</v>
@@ -9019,7 +9019,7 @@
         <v>560</v>
       </c>
       <c r="B302" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="C302">
         <v>3</v>
@@ -9039,7 +9039,7 @@
         <v>562</v>
       </c>
       <c r="B303" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C303">
         <v>5</v>
@@ -9073,7 +9073,7 @@
         <v>564</v>
       </c>
       <c r="B305" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C305">
         <v>5</v>
@@ -9107,7 +9107,7 @@
         <v>221</v>
       </c>
       <c r="B307" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="C307">
         <v>1</v>

</xml_diff>